<commit_message>
pseudo stash for Jules
</commit_message>
<xml_diff>
--- a/paper/Table_S1.xlsx
+++ b/paper/Table_S1.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="246">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="300">
   <si>
     <t xml:space="preserve">Country</t>
   </si>
@@ -65,486 +65,606 @@
     <t xml:space="preserve">(-1,650; 4,130)</t>
   </si>
   <si>
+    <t xml:space="preserve">-1,415</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(-10,670; 6,885)</t>
+  </si>
+  <si>
     <t xml:space="preserve">-410</t>
   </si>
   <si>
     <t xml:space="preserve">(-3,405; 2,510)</t>
   </si>
   <si>
+    <t xml:space="preserve">3,455</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(705; 6,120)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3,380</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3,360</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(605; 6,015)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-525</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(-9,665; 7,890)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1,790</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(-1,110; 4,565)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1,920</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(-1,265; 5,010)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1,975</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1,585</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(-1,605; 4,520)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-12,310</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(-26,845; 570)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">990</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(-2,140; 4,045)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3,810</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(1,155; 6,395)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3,630</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3,855</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(1,175; 6,505)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-11,490</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(-21,800; -2,175)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1,905</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(-925; 4,630)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">24,730</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(21,925; 27,455)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">24,460</t>
+  </si>
+  <si>
+    <t xml:space="preserve">24,625</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(21,690; 27,465)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11,965</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(1,835; 21,075)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">23,705</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(20,540; 26,705)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3,730</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(510; 6,835)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3,820</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3,700</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(515; 6,790)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-25,935</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(-42,040; -11,745)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(200; 6,540)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1,535</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(-775; 3,750)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1,555</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1,470</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(-865; 3,725)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-8,290</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(-15,635; -1,405)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(-630; 3,710)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-920</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(-3,680; 1,805)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-1,200</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-1,035</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(-3,835; 1,675)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-10,905</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(-19,500; -2,965)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-25</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(-2,440; 2,295)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-3,705</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(-6,950; -605)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-3,360</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-3,190</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(-6,315; -185)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-32,105</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(-46,645; -18,910)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-2,760</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(-5,095; -380)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">165</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(-3,210; 3,400)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">280</t>
+  </si>
+  <si>
+    <t xml:space="preserve">320</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(-2,950; 3,460)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-12,495</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(-21,095; -4,055)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">600</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(-1,865; 2,975)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8,430</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(5,255; 11,450)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8,810</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8,685</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(5,575; 11,675)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-5,110</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(-13,425; 2,510)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7,360</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(4,395; 10,240)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-1,000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(-3,085; 955)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-845</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-715</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(-2,735; 1,220)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-9,630</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(-16,685; -3,065)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-925</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(-3,280; 1,375)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sweden</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2,495</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(-1,400; 6,155)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2,785</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2,540</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(-1,280; 6,290)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-1,710</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(-11,930; 7,590)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-1,125</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(-5,425; 2,960)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(4,870; 12,575)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8,720</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8,525</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(4,475; 12,495)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3,115</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(-7,690; 13,170)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7,060</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(2,930; 11,055)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5,295</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(800; 9,480)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6,365</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5,570</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(1,045; 9,800)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-16,280</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(-34,020; -870)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5,875</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(1,405; 10,255)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-2,640</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(-7,970; 2,330)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-2,980</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-2,865</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(-8,140; 2,105)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-3,355</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(-14,570; 6,390)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-645</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(-4,165; 2,725)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">25,935</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(20,595; 31,085)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">25,505</t>
+  </si>
+  <si>
+    <t xml:space="preserve">25,695</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(20,310; 30,885)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">22,390</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(11,965; 32,040)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">27,700</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(23,945; 31,250)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7,245</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(1,180; 12,965)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8,260</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7,140</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(1,020; 12,835)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-11,745</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(-28,035; 2,690)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7,395</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(3,625; 11,080)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1,080</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(-2,395; 4,445)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1,450</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(-2,085; 4,910)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-11,945</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(-20,990; -3,515)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">880</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(-2,410; 4,065)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2,760</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(100; 5,340)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3,040</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2,990</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(395; 5,515)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-8,150</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(-16,645; 70)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3,135</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(-470; 6,575)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-360</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(-3,505; 2,720)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1,040</t>
+  </si>
+  <si>
+    <t xml:space="preserve">620</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(-2,465; 3,605)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-41,850</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(-59,685; -25,600)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-800</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(-4,875; 3,060)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-4,365</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(-8,015; -795)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-4,390</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-4,255</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(-7,810; -730)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-13,045</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(-22,010; -4,515)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-4,380</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(-7,125; -1,695)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7,655</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(4,200; 10,985)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8,465</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8,405</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(4,960; 11,690)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-4,225</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(-12,640; 3,910)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2,600</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(-690; 5,750)</t>
+  </si>
+  <si>
     <t xml:space="preserve">--</t>
   </si>
   <si>
-    <t xml:space="preserve">3,455</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(705; 6,120)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3,380</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3,360</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(605; 6,015)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1,790</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(-1,110; 4,565)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1,920</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(-1,265; 5,010)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1,975</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1,585</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(-1,605; 4,520)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">990</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(-2,140; 4,045)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3,810</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(1,155; 6,395)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3,630</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3,855</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(1,175; 6,505)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1,905</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(-925; 4,630)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">24,730</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(21,925; 27,455)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">24,460</t>
-  </si>
-  <si>
-    <t xml:space="preserve">24,625</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(21,690; 27,465)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">23,705</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(20,540; 26,705)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3,730</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(510; 6,835)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3,820</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3,700</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(515; 6,790)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(200; 6,540)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1,535</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(-775; 3,750)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1,555</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1,470</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(-865; 3,725)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(-630; 3,710)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-920</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(-3,680; 1,805)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-1,200</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-1,035</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(-3,835; 1,675)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-25</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(-2,440; 2,295)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-3,705</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(-6,950; -605)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-3,360</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-3,190</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(-6,315; -185)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-2,760</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(-5,095; -380)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">165</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(-3,210; 3,400)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">280</t>
-  </si>
-  <si>
-    <t xml:space="preserve">320</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(-2,950; 3,460)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">600</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(-1,865; 2,975)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">8,430</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(5,255; 11,450)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">8,810</t>
-  </si>
-  <si>
-    <t xml:space="preserve">8,685</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(5,575; 11,675)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">7,360</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(4,395; 10,240)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">8,585</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(5,435; 11,595)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-1,000</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(-3,085; 955)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-845</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-715</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(-2,735; 1,220)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-925</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(-3,280; 1,375)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-1,225</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(-3,320; 790)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sweden</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2,495</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(-1,400; 6,155)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2,785</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2,540</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(-1,280; 6,290)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-1,125</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(-5,425; 2,960)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(4,870; 12,575)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">8,720</t>
-  </si>
-  <si>
-    <t xml:space="preserve">8,525</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(4,475; 12,495)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">7,060</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(2,930; 11,055)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5,295</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(800; 9,480)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6,365</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5,570</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(1,045; 9,800)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5,875</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(1,405; 10,255)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-2,640</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(-7,970; 2,330)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-2,980</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-2,865</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(-8,140; 2,105)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-645</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(-4,165; 2,725)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">25,935</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(20,595; 31,085)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">25,505</t>
-  </si>
-  <si>
-    <t xml:space="preserve">25,695</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(20,310; 30,885)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">27,700</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(23,945; 31,250)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">7,245</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(1,180; 12,965)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">8,260</t>
-  </si>
-  <si>
-    <t xml:space="preserve">7,140</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(1,020; 12,835)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">7,395</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(3,625; 11,080)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1,080</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(-2,395; 4,445)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1,450</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(-2,085; 4,910)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">880</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(-2,410; 4,065)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2,760</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(100; 5,340)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3,040</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2,990</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(395; 5,515)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3,135</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(-470; 6,575)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-360</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(-3,505; 2,720)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1,040</t>
-  </si>
-  <si>
-    <t xml:space="preserve">620</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(-2,465; 3,605)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-800</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(-4,875; 3,060)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-4,365</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(-8,015; -795)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-4,390</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-4,255</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(-7,810; -730)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-4,380</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(-7,125; -1,695)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">7,655</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(4,200; 10,985)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">8,465</t>
-  </si>
-  <si>
-    <t xml:space="preserve">8,405</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(4,960; 11,690)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2,600</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(-690; 5,750)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">8,130</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(4,650; 11,520)</t>
-  </si>
-  <si>
     <t xml:space="preserve">1,700</t>
   </si>
   <si>
@@ -572,6 +692,12 @@
     <t xml:space="preserve">(-13,400; 36,025)</t>
   </si>
   <si>
+    <t xml:space="preserve">31,205</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(-6,895; 66,725)</t>
+  </si>
+  <si>
     <t xml:space="preserve">20,950</t>
   </si>
   <si>
@@ -593,6 +719,12 @@
     <t xml:space="preserve">(214,035; 264,175)</t>
   </si>
   <si>
+    <t xml:space="preserve">265,120</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(220,910; 306,775)</t>
+  </si>
+  <si>
     <t xml:space="preserve">28,835</t>
   </si>
   <si>
@@ -608,6 +740,12 @@
     <t xml:space="preserve">(-4,940; 49,265)</t>
   </si>
   <si>
+    <t xml:space="preserve">25,970</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(-52,320; 97,395)</t>
+  </si>
+  <si>
     <t xml:space="preserve">45,235</t>
   </si>
   <si>
@@ -629,6 +767,12 @@
     <t xml:space="preserve">(10,205; 54,805)</t>
   </si>
   <si>
+    <t xml:space="preserve">-73,990</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(-143,425; -12,155)</t>
+  </si>
+  <si>
     <t xml:space="preserve">30,730</t>
   </si>
   <si>
@@ -650,6 +794,12 @@
     <t xml:space="preserve">(-4,495; 27,310)</t>
   </si>
   <si>
+    <t xml:space="preserve">-29,977,380</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(-119,706,000; -8,050)</t>
+  </si>
+  <si>
     <t xml:space="preserve">21,360</t>
   </si>
   <si>
@@ -671,6 +821,12 @@
     <t xml:space="preserve">(-48,745; -9,615)</t>
   </si>
   <si>
+    <t xml:space="preserve">-107,725</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(-191,465; -34,400)</t>
+  </si>
+  <si>
     <t xml:space="preserve">-27,265</t>
   </si>
   <si>
@@ -692,6 +848,12 @@
     <t xml:space="preserve">(-41,320; 1,025)</t>
   </si>
   <si>
+    <t xml:space="preserve">-56,115</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(-117,505; -260)</t>
+  </si>
+  <si>
     <t xml:space="preserve">-10,460</t>
   </si>
   <si>
@@ -713,18 +875,18 @@
     <t xml:space="preserve">(44,510; 85,625)</t>
   </si>
   <si>
+    <t xml:space="preserve">-11,300</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(-74,995; 45,780)</t>
+  </si>
+  <si>
     <t xml:space="preserve">69,225</t>
   </si>
   <si>
     <t xml:space="preserve">(47,980; 89,670)</t>
   </si>
   <si>
-    <t xml:space="preserve">69,420</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(48,860; 89,285)</t>
-  </si>
-  <si>
     <t xml:space="preserve">10,865</t>
   </si>
   <si>
@@ -740,16 +902,16 @@
     <t xml:space="preserve">(-3,525; 24,785)</t>
   </si>
   <si>
+    <t xml:space="preserve">-41,955</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(-85,995; -1,680)</t>
+  </si>
+  <si>
     <t xml:space="preserve">14,245</t>
   </si>
   <si>
     <t xml:space="preserve">(-265; 28,120)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">8,035</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(-6,420; 22,245)</t>
   </si>
 </sst>
 </file>
@@ -1148,7 +1310,7 @@
         <v>19</v>
       </c>
       <c r="K2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3">
@@ -1159,31 +1321,31 @@
         <v>1890</v>
       </c>
       <c r="C3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="H3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="I3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="J3" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="K3" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4">
@@ -1194,31 +1356,31 @@
         <v>1891</v>
       </c>
       <c r="C4" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="D4" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="E4" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="F4" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="G4" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="H4" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="I4" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="J4" t="s">
-        <v>19</v>
+        <v>37</v>
       </c>
       <c r="K4" t="s">
-        <v>19</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5">
@@ -1229,31 +1391,31 @@
         <v>1917</v>
       </c>
       <c r="C5" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="D5" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="E5" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="F5" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="G5" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="H5" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="I5" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="J5" t="s">
-        <v>19</v>
+        <v>46</v>
       </c>
       <c r="K5" t="s">
-        <v>19</v>
+        <v>47</v>
       </c>
     </row>
     <row r="6">
@@ -1264,31 +1426,31 @@
         <v>1918</v>
       </c>
       <c r="C6" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="D6" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="E6" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="F6" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="G6" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="H6" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
       <c r="I6" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="J6" t="s">
-        <v>19</v>
+        <v>55</v>
       </c>
       <c r="K6" t="s">
-        <v>19</v>
+        <v>56</v>
       </c>
     </row>
     <row r="7">
@@ -1299,31 +1461,31 @@
         <v>1919</v>
       </c>
       <c r="C7" t="s">
-        <v>48</v>
+        <v>57</v>
       </c>
       <c r="D7" t="s">
-        <v>49</v>
+        <v>58</v>
       </c>
       <c r="E7" t="s">
-        <v>50</v>
+        <v>59</v>
       </c>
       <c r="F7" t="s">
-        <v>51</v>
+        <v>60</v>
       </c>
       <c r="G7" t="s">
-        <v>52</v>
+        <v>61</v>
       </c>
       <c r="H7" t="s">
-        <v>20</v>
+        <v>62</v>
       </c>
       <c r="I7" t="s">
-        <v>53</v>
+        <v>63</v>
       </c>
       <c r="J7" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="K7" t="s">
-        <v>19</v>
+        <v>64</v>
       </c>
     </row>
     <row r="8">
@@ -1334,31 +1496,31 @@
         <v>1956</v>
       </c>
       <c r="C8" t="s">
-        <v>54</v>
+        <v>65</v>
       </c>
       <c r="D8" t="s">
-        <v>55</v>
+        <v>66</v>
       </c>
       <c r="E8" t="s">
-        <v>56</v>
+        <v>67</v>
       </c>
       <c r="F8" t="s">
-        <v>57</v>
+        <v>68</v>
       </c>
       <c r="G8" t="s">
-        <v>58</v>
+        <v>69</v>
       </c>
       <c r="H8" t="s">
-        <v>56</v>
+        <v>70</v>
       </c>
       <c r="I8" t="s">
-        <v>59</v>
+        <v>71</v>
       </c>
       <c r="J8" t="s">
-        <v>19</v>
+        <v>67</v>
       </c>
       <c r="K8" t="s">
-        <v>19</v>
+        <v>72</v>
       </c>
     </row>
     <row r="9">
@@ -1369,31 +1531,31 @@
         <v>1957</v>
       </c>
       <c r="C9" t="s">
-        <v>60</v>
+        <v>73</v>
       </c>
       <c r="D9" t="s">
-        <v>61</v>
+        <v>74</v>
       </c>
       <c r="E9" t="s">
-        <v>62</v>
+        <v>75</v>
       </c>
       <c r="F9" t="s">
-        <v>63</v>
+        <v>76</v>
       </c>
       <c r="G9" t="s">
-        <v>64</v>
+        <v>77</v>
       </c>
       <c r="H9" t="s">
-        <v>65</v>
+        <v>78</v>
       </c>
       <c r="I9" t="s">
-        <v>66</v>
+        <v>79</v>
       </c>
       <c r="J9" t="s">
-        <v>19</v>
+        <v>80</v>
       </c>
       <c r="K9" t="s">
-        <v>19</v>
+        <v>81</v>
       </c>
     </row>
     <row r="10">
@@ -1404,31 +1566,31 @@
         <v>1958</v>
       </c>
       <c r="C10" t="s">
-        <v>67</v>
+        <v>82</v>
       </c>
       <c r="D10" t="s">
-        <v>68</v>
+        <v>83</v>
       </c>
       <c r="E10" t="s">
-        <v>69</v>
+        <v>84</v>
       </c>
       <c r="F10" t="s">
-        <v>70</v>
+        <v>85</v>
       </c>
       <c r="G10" t="s">
-        <v>71</v>
+        <v>86</v>
       </c>
       <c r="H10" t="s">
-        <v>72</v>
+        <v>87</v>
       </c>
       <c r="I10" t="s">
-        <v>73</v>
+        <v>88</v>
       </c>
       <c r="J10" t="s">
-        <v>19</v>
+        <v>89</v>
       </c>
       <c r="K10" t="s">
-        <v>19</v>
+        <v>90</v>
       </c>
     </row>
     <row r="11">
@@ -1439,31 +1601,31 @@
         <v>2019</v>
       </c>
       <c r="C11" t="s">
-        <v>74</v>
+        <v>91</v>
       </c>
       <c r="D11" t="s">
-        <v>75</v>
+        <v>92</v>
       </c>
       <c r="E11" t="s">
-        <v>76</v>
+        <v>93</v>
       </c>
       <c r="F11" t="s">
-        <v>77</v>
+        <v>94</v>
       </c>
       <c r="G11" t="s">
-        <v>78</v>
+        <v>95</v>
       </c>
       <c r="H11" t="s">
-        <v>79</v>
+        <v>96</v>
       </c>
       <c r="I11" t="s">
-        <v>80</v>
+        <v>97</v>
       </c>
       <c r="J11" t="s">
-        <v>19</v>
+        <v>98</v>
       </c>
       <c r="K11" t="s">
-        <v>19</v>
+        <v>99</v>
       </c>
     </row>
     <row r="12">
@@ -1474,31 +1636,31 @@
         <v>2020</v>
       </c>
       <c r="C12" t="s">
-        <v>81</v>
+        <v>100</v>
       </c>
       <c r="D12" t="s">
-        <v>82</v>
+        <v>101</v>
       </c>
       <c r="E12" t="s">
-        <v>83</v>
+        <v>102</v>
       </c>
       <c r="F12" t="s">
-        <v>84</v>
+        <v>103</v>
       </c>
       <c r="G12" t="s">
-        <v>85</v>
+        <v>104</v>
       </c>
       <c r="H12" t="s">
-        <v>86</v>
+        <v>105</v>
       </c>
       <c r="I12" t="s">
-        <v>87</v>
+        <v>106</v>
       </c>
       <c r="J12" t="s">
-        <v>88</v>
+        <v>107</v>
       </c>
       <c r="K12" t="s">
-        <v>89</v>
+        <v>108</v>
       </c>
     </row>
     <row r="13">
@@ -1509,766 +1671,766 @@
         <v>2021</v>
       </c>
       <c r="C13" t="s">
-        <v>90</v>
+        <v>109</v>
       </c>
       <c r="D13" t="s">
-        <v>91</v>
+        <v>110</v>
       </c>
       <c r="E13" t="s">
-        <v>92</v>
+        <v>111</v>
       </c>
       <c r="F13" t="s">
-        <v>93</v>
+        <v>112</v>
       </c>
       <c r="G13" t="s">
-        <v>94</v>
+        <v>113</v>
       </c>
       <c r="H13" t="s">
-        <v>95</v>
+        <v>114</v>
       </c>
       <c r="I13" t="s">
-        <v>96</v>
+        <v>115</v>
       </c>
       <c r="J13" t="s">
-        <v>97</v>
+        <v>116</v>
       </c>
       <c r="K13" t="s">
-        <v>98</v>
+        <v>117</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>99</v>
+        <v>118</v>
       </c>
       <c r="B14" t="n">
         <v>1889</v>
       </c>
       <c r="C14" t="s">
-        <v>100</v>
+        <v>119</v>
       </c>
       <c r="D14" t="s">
-        <v>101</v>
+        <v>120</v>
       </c>
       <c r="E14" t="s">
-        <v>102</v>
+        <v>121</v>
       </c>
       <c r="F14" t="s">
-        <v>103</v>
+        <v>122</v>
       </c>
       <c r="G14" t="s">
-        <v>104</v>
+        <v>123</v>
       </c>
       <c r="H14" t="s">
-        <v>105</v>
+        <v>124</v>
       </c>
       <c r="I14" t="s">
-        <v>106</v>
+        <v>125</v>
       </c>
       <c r="J14" t="s">
-        <v>19</v>
+        <v>126</v>
       </c>
       <c r="K14" t="s">
-        <v>19</v>
+        <v>127</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>99</v>
+        <v>118</v>
       </c>
       <c r="B15" t="n">
         <v>1890</v>
       </c>
       <c r="C15" t="s">
-        <v>83</v>
+        <v>102</v>
       </c>
       <c r="D15" t="s">
-        <v>107</v>
+        <v>128</v>
       </c>
       <c r="E15" t="s">
-        <v>108</v>
+        <v>129</v>
       </c>
       <c r="F15" t="s">
-        <v>109</v>
+        <v>130</v>
       </c>
       <c r="G15" t="s">
-        <v>110</v>
+        <v>131</v>
       </c>
       <c r="H15" t="s">
-        <v>111</v>
+        <v>132</v>
       </c>
       <c r="I15" t="s">
-        <v>112</v>
+        <v>133</v>
       </c>
       <c r="J15" t="s">
-        <v>19</v>
+        <v>134</v>
       </c>
       <c r="K15" t="s">
-        <v>19</v>
+        <v>135</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>99</v>
+        <v>118</v>
       </c>
       <c r="B16" t="n">
         <v>1891</v>
       </c>
       <c r="C16" t="s">
-        <v>113</v>
+        <v>136</v>
       </c>
       <c r="D16" t="s">
-        <v>114</v>
+        <v>137</v>
       </c>
       <c r="E16" t="s">
-        <v>115</v>
+        <v>138</v>
       </c>
       <c r="F16" t="s">
-        <v>116</v>
+        <v>139</v>
       </c>
       <c r="G16" t="s">
-        <v>117</v>
+        <v>140</v>
       </c>
       <c r="H16" t="s">
-        <v>118</v>
+        <v>141</v>
       </c>
       <c r="I16" t="s">
-        <v>119</v>
+        <v>142</v>
       </c>
       <c r="J16" t="s">
-        <v>19</v>
+        <v>143</v>
       </c>
       <c r="K16" t="s">
-        <v>19</v>
+        <v>144</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>99</v>
+        <v>118</v>
       </c>
       <c r="B17" t="n">
         <v>1917</v>
       </c>
       <c r="C17" t="s">
-        <v>120</v>
+        <v>145</v>
       </c>
       <c r="D17" t="s">
-        <v>121</v>
+        <v>146</v>
       </c>
       <c r="E17" t="s">
-        <v>122</v>
+        <v>147</v>
       </c>
       <c r="F17" t="s">
-        <v>123</v>
+        <v>148</v>
       </c>
       <c r="G17" t="s">
-        <v>124</v>
+        <v>149</v>
       </c>
       <c r="H17" t="s">
-        <v>125</v>
+        <v>150</v>
       </c>
       <c r="I17" t="s">
-        <v>126</v>
+        <v>151</v>
       </c>
       <c r="J17" t="s">
-        <v>19</v>
+        <v>152</v>
       </c>
       <c r="K17" t="s">
-        <v>19</v>
+        <v>153</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>99</v>
+        <v>118</v>
       </c>
       <c r="B18" t="n">
         <v>1918</v>
       </c>
       <c r="C18" t="s">
-        <v>127</v>
+        <v>154</v>
       </c>
       <c r="D18" t="s">
-        <v>128</v>
+        <v>155</v>
       </c>
       <c r="E18" t="s">
-        <v>129</v>
+        <v>156</v>
       </c>
       <c r="F18" t="s">
-        <v>130</v>
+        <v>157</v>
       </c>
       <c r="G18" t="s">
-        <v>131</v>
+        <v>158</v>
       </c>
       <c r="H18" t="s">
-        <v>132</v>
+        <v>159</v>
       </c>
       <c r="I18" t="s">
-        <v>133</v>
+        <v>160</v>
       </c>
       <c r="J18" t="s">
-        <v>19</v>
+        <v>161</v>
       </c>
       <c r="K18" t="s">
-        <v>19</v>
+        <v>162</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>99</v>
+        <v>118</v>
       </c>
       <c r="B19" t="n">
         <v>1919</v>
       </c>
       <c r="C19" t="s">
-        <v>134</v>
+        <v>163</v>
       </c>
       <c r="D19" t="s">
-        <v>135</v>
+        <v>164</v>
       </c>
       <c r="E19" t="s">
-        <v>136</v>
+        <v>165</v>
       </c>
       <c r="F19" t="s">
-        <v>137</v>
+        <v>166</v>
       </c>
       <c r="G19" t="s">
-        <v>138</v>
+        <v>167</v>
       </c>
       <c r="H19" t="s">
-        <v>139</v>
+        <v>168</v>
       </c>
       <c r="I19" t="s">
-        <v>140</v>
+        <v>169</v>
       </c>
       <c r="J19" t="s">
-        <v>19</v>
+        <v>170</v>
       </c>
       <c r="K19" t="s">
-        <v>19</v>
+        <v>171</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>99</v>
+        <v>118</v>
       </c>
       <c r="B20" t="n">
         <v>1956</v>
       </c>
       <c r="C20" t="s">
-        <v>141</v>
+        <v>172</v>
       </c>
       <c r="D20" t="s">
-        <v>142</v>
+        <v>173</v>
       </c>
       <c r="E20" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="F20" t="s">
-        <v>143</v>
+        <v>174</v>
       </c>
       <c r="G20" t="s">
-        <v>144</v>
+        <v>175</v>
       </c>
       <c r="H20" t="s">
-        <v>145</v>
+        <v>176</v>
       </c>
       <c r="I20" t="s">
-        <v>146</v>
+        <v>177</v>
       </c>
       <c r="J20" t="s">
-        <v>19</v>
+        <v>178</v>
       </c>
       <c r="K20" t="s">
-        <v>19</v>
+        <v>179</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>99</v>
+        <v>118</v>
       </c>
       <c r="B21" t="n">
         <v>1957</v>
       </c>
       <c r="C21" t="s">
-        <v>147</v>
+        <v>180</v>
       </c>
       <c r="D21" t="s">
-        <v>148</v>
+        <v>181</v>
       </c>
       <c r="E21" t="s">
-        <v>149</v>
+        <v>182</v>
       </c>
       <c r="F21" t="s">
-        <v>150</v>
+        <v>183</v>
       </c>
       <c r="G21" t="s">
-        <v>151</v>
+        <v>184</v>
       </c>
       <c r="H21" t="s">
-        <v>152</v>
+        <v>185</v>
       </c>
       <c r="I21" t="s">
-        <v>153</v>
+        <v>186</v>
       </c>
       <c r="J21" t="s">
-        <v>19</v>
+        <v>187</v>
       </c>
       <c r="K21" t="s">
-        <v>19</v>
+        <v>188</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>99</v>
+        <v>118</v>
       </c>
       <c r="B22" t="n">
         <v>1958</v>
       </c>
       <c r="C22" t="s">
-        <v>154</v>
+        <v>189</v>
       </c>
       <c r="D22" t="s">
-        <v>155</v>
+        <v>190</v>
       </c>
       <c r="E22" t="s">
-        <v>156</v>
+        <v>191</v>
       </c>
       <c r="F22" t="s">
-        <v>157</v>
+        <v>192</v>
       </c>
       <c r="G22" t="s">
-        <v>158</v>
+        <v>193</v>
       </c>
       <c r="H22" t="s">
-        <v>159</v>
+        <v>194</v>
       </c>
       <c r="I22" t="s">
-        <v>160</v>
+        <v>195</v>
       </c>
       <c r="J22" t="s">
-        <v>19</v>
+        <v>196</v>
       </c>
       <c r="K22" t="s">
-        <v>19</v>
+        <v>197</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>99</v>
+        <v>118</v>
       </c>
       <c r="B23" t="n">
         <v>2019</v>
       </c>
       <c r="C23" t="s">
-        <v>161</v>
+        <v>198</v>
       </c>
       <c r="D23" t="s">
-        <v>162</v>
+        <v>199</v>
       </c>
       <c r="E23" t="s">
-        <v>163</v>
+        <v>200</v>
       </c>
       <c r="F23" t="s">
-        <v>164</v>
+        <v>201</v>
       </c>
       <c r="G23" t="s">
-        <v>165</v>
+        <v>202</v>
       </c>
       <c r="H23" t="s">
-        <v>166</v>
+        <v>203</v>
       </c>
       <c r="I23" t="s">
-        <v>167</v>
+        <v>204</v>
       </c>
       <c r="J23" t="s">
-        <v>19</v>
+        <v>205</v>
       </c>
       <c r="K23" t="s">
-        <v>19</v>
+        <v>206</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>99</v>
+        <v>118</v>
       </c>
       <c r="B24" t="n">
         <v>2020</v>
       </c>
       <c r="C24" t="s">
-        <v>168</v>
+        <v>207</v>
       </c>
       <c r="D24" t="s">
-        <v>169</v>
+        <v>208</v>
       </c>
       <c r="E24" t="s">
-        <v>170</v>
+        <v>209</v>
       </c>
       <c r="F24" t="s">
-        <v>171</v>
+        <v>210</v>
       </c>
       <c r="G24" t="s">
-        <v>172</v>
+        <v>211</v>
       </c>
       <c r="H24" t="s">
-        <v>173</v>
+        <v>212</v>
       </c>
       <c r="I24" t="s">
-        <v>174</v>
+        <v>213</v>
       </c>
       <c r="J24" t="s">
-        <v>175</v>
+        <v>214</v>
       </c>
       <c r="K24" t="s">
-        <v>176</v>
+        <v>215</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>99</v>
+        <v>118</v>
       </c>
       <c r="B25" t="n">
         <v>2021</v>
       </c>
       <c r="C25" t="s">
-        <v>19</v>
+        <v>216</v>
       </c>
       <c r="D25" t="s">
-        <v>19</v>
+        <v>216</v>
       </c>
       <c r="E25" t="s">
-        <v>177</v>
+        <v>217</v>
       </c>
       <c r="F25" t="s">
-        <v>178</v>
+        <v>218</v>
       </c>
       <c r="G25" t="s">
-        <v>179</v>
+        <v>219</v>
       </c>
       <c r="H25" t="s">
-        <v>19</v>
+        <v>216</v>
       </c>
       <c r="I25" t="s">
-        <v>19</v>
+        <v>216</v>
       </c>
       <c r="J25" t="s">
-        <v>19</v>
+        <v>216</v>
       </c>
       <c r="K25" t="s">
-        <v>19</v>
+        <v>216</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>180</v>
+        <v>220</v>
       </c>
       <c r="B26" t="n">
         <v>1917</v>
       </c>
       <c r="C26" t="s">
-        <v>181</v>
+        <v>221</v>
       </c>
       <c r="D26" t="s">
-        <v>182</v>
+        <v>222</v>
       </c>
       <c r="E26" t="s">
-        <v>183</v>
+        <v>223</v>
       </c>
       <c r="F26" t="s">
-        <v>184</v>
+        <v>224</v>
       </c>
       <c r="G26" t="s">
-        <v>185</v>
+        <v>225</v>
       </c>
       <c r="H26" t="s">
-        <v>186</v>
+        <v>226</v>
       </c>
       <c r="I26" t="s">
-        <v>187</v>
+        <v>227</v>
       </c>
       <c r="J26" t="s">
-        <v>19</v>
+        <v>228</v>
       </c>
       <c r="K26" t="s">
-        <v>19</v>
+        <v>229</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>180</v>
+        <v>220</v>
       </c>
       <c r="B27" t="n">
         <v>1918</v>
       </c>
       <c r="C27" t="s">
-        <v>188</v>
+        <v>230</v>
       </c>
       <c r="D27" t="s">
-        <v>189</v>
+        <v>231</v>
       </c>
       <c r="E27" t="s">
-        <v>190</v>
+        <v>232</v>
       </c>
       <c r="F27" t="s">
-        <v>191</v>
+        <v>233</v>
       </c>
       <c r="G27" t="s">
-        <v>192</v>
+        <v>234</v>
       </c>
       <c r="H27" t="s">
-        <v>188</v>
+        <v>235</v>
       </c>
       <c r="I27" t="s">
-        <v>189</v>
+        <v>236</v>
       </c>
       <c r="J27" t="s">
-        <v>19</v>
+        <v>230</v>
       </c>
       <c r="K27" t="s">
-        <v>19</v>
+        <v>231</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>180</v>
+        <v>220</v>
       </c>
       <c r="B28" t="n">
         <v>1919</v>
       </c>
       <c r="C28" t="s">
-        <v>193</v>
+        <v>237</v>
       </c>
       <c r="D28" t="s">
-        <v>194</v>
+        <v>238</v>
       </c>
       <c r="E28" t="s">
-        <v>195</v>
+        <v>239</v>
       </c>
       <c r="F28" t="s">
-        <v>196</v>
+        <v>240</v>
       </c>
       <c r="G28" t="s">
-        <v>197</v>
+        <v>241</v>
       </c>
       <c r="H28" t="s">
-        <v>198</v>
+        <v>242</v>
       </c>
       <c r="I28" t="s">
-        <v>199</v>
+        <v>243</v>
       </c>
       <c r="J28" t="s">
-        <v>19</v>
+        <v>244</v>
       </c>
       <c r="K28" t="s">
-        <v>19</v>
+        <v>245</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>180</v>
+        <v>220</v>
       </c>
       <c r="B29" t="n">
         <v>1956</v>
       </c>
       <c r="C29" t="s">
-        <v>200</v>
+        <v>246</v>
       </c>
       <c r="D29" t="s">
-        <v>201</v>
+        <v>247</v>
       </c>
       <c r="E29" t="s">
-        <v>202</v>
+        <v>248</v>
       </c>
       <c r="F29" t="s">
-        <v>203</v>
+        <v>249</v>
       </c>
       <c r="G29" t="s">
-        <v>204</v>
+        <v>250</v>
       </c>
       <c r="H29" t="s">
-        <v>205</v>
+        <v>251</v>
       </c>
       <c r="I29" t="s">
-        <v>206</v>
+        <v>252</v>
       </c>
       <c r="J29" t="s">
-        <v>19</v>
+        <v>253</v>
       </c>
       <c r="K29" t="s">
-        <v>19</v>
+        <v>254</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>180</v>
+        <v>220</v>
       </c>
       <c r="B30" t="n">
         <v>1957</v>
       </c>
       <c r="C30" t="s">
-        <v>207</v>
+        <v>255</v>
       </c>
       <c r="D30" t="s">
-        <v>208</v>
+        <v>256</v>
       </c>
       <c r="E30" t="s">
-        <v>209</v>
+        <v>257</v>
       </c>
       <c r="F30" t="s">
-        <v>210</v>
+        <v>258</v>
       </c>
       <c r="G30" t="s">
-        <v>211</v>
+        <v>259</v>
       </c>
       <c r="H30" t="s">
-        <v>212</v>
+        <v>260</v>
       </c>
       <c r="I30" t="s">
-        <v>213</v>
+        <v>261</v>
       </c>
       <c r="J30" t="s">
-        <v>19</v>
+        <v>262</v>
       </c>
       <c r="K30" t="s">
-        <v>19</v>
+        <v>263</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>180</v>
+        <v>220</v>
       </c>
       <c r="B31" t="n">
         <v>1958</v>
       </c>
       <c r="C31" t="s">
-        <v>214</v>
+        <v>264</v>
       </c>
       <c r="D31" t="s">
-        <v>215</v>
+        <v>265</v>
       </c>
       <c r="E31" t="s">
-        <v>216</v>
+        <v>266</v>
       </c>
       <c r="F31" t="s">
-        <v>217</v>
+        <v>267</v>
       </c>
       <c r="G31" t="s">
-        <v>218</v>
+        <v>268</v>
       </c>
       <c r="H31" t="s">
-        <v>219</v>
+        <v>269</v>
       </c>
       <c r="I31" t="s">
-        <v>220</v>
+        <v>270</v>
       </c>
       <c r="J31" t="s">
-        <v>19</v>
+        <v>271</v>
       </c>
       <c r="K31" t="s">
-        <v>19</v>
+        <v>272</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>180</v>
+        <v>220</v>
       </c>
       <c r="B32" t="n">
         <v>2019</v>
       </c>
       <c r="C32" t="s">
-        <v>221</v>
+        <v>273</v>
       </c>
       <c r="D32" t="s">
-        <v>222</v>
+        <v>274</v>
       </c>
       <c r="E32" t="s">
-        <v>223</v>
+        <v>275</v>
       </c>
       <c r="F32" t="s">
-        <v>224</v>
+        <v>276</v>
       </c>
       <c r="G32" t="s">
-        <v>225</v>
+        <v>277</v>
       </c>
       <c r="H32" t="s">
-        <v>226</v>
+        <v>278</v>
       </c>
       <c r="I32" t="s">
-        <v>227</v>
+        <v>279</v>
       </c>
       <c r="J32" t="s">
-        <v>19</v>
+        <v>280</v>
       </c>
       <c r="K32" t="s">
-        <v>19</v>
+        <v>281</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>180</v>
+        <v>220</v>
       </c>
       <c r="B33" t="n">
         <v>2020</v>
       </c>
       <c r="C33" t="s">
-        <v>228</v>
+        <v>282</v>
       </c>
       <c r="D33" t="s">
-        <v>229</v>
+        <v>283</v>
       </c>
       <c r="E33" t="s">
-        <v>230</v>
+        <v>284</v>
       </c>
       <c r="F33" t="s">
-        <v>231</v>
+        <v>285</v>
       </c>
       <c r="G33" t="s">
-        <v>232</v>
+        <v>286</v>
       </c>
       <c r="H33" t="s">
-        <v>233</v>
+        <v>287</v>
       </c>
       <c r="I33" t="s">
-        <v>234</v>
+        <v>288</v>
       </c>
       <c r="J33" t="s">
-        <v>235</v>
+        <v>289</v>
       </c>
       <c r="K33" t="s">
-        <v>236</v>
+        <v>290</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>180</v>
+        <v>220</v>
       </c>
       <c r="B34" t="n">
         <v>2021</v>
       </c>
       <c r="C34" t="s">
-        <v>237</v>
+        <v>291</v>
       </c>
       <c r="D34" t="s">
-        <v>238</v>
+        <v>292</v>
       </c>
       <c r="E34" t="s">
-        <v>239</v>
+        <v>293</v>
       </c>
       <c r="F34" t="s">
-        <v>240</v>
+        <v>294</v>
       </c>
       <c r="G34" t="s">
-        <v>241</v>
+        <v>295</v>
       </c>
       <c r="H34" t="s">
-        <v>242</v>
+        <v>296</v>
       </c>
       <c r="I34" t="s">
-        <v>243</v>
+        <v>297</v>
       </c>
       <c r="J34" t="s">
-        <v>244</v>
+        <v>298</v>
       </c>
       <c r="K34" t="s">
-        <v>245</v>
+        <v>299</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
checks of trim models
</commit_message>
<xml_diff>
--- a/paper/Table_S1.xlsx
+++ b/paper/Table_S1.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="300">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="298">
   <si>
     <t xml:space="preserve">Country</t>
   </si>
@@ -65,10 +65,10 @@
     <t xml:space="preserve">(-1,650; 4,130)</t>
   </si>
   <si>
-    <t xml:space="preserve">-1,415</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(-10,670; 6,885)</t>
+    <t xml:space="preserve">1,680</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(-865; 4,190)</t>
   </si>
   <si>
     <t xml:space="preserve">-410</t>
@@ -92,10 +92,10 @@
     <t xml:space="preserve">(605; 6,015)</t>
   </si>
   <si>
-    <t xml:space="preserve">-525</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(-9,665; 7,890)</t>
+    <t xml:space="preserve">2,395</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(-310; 5,020)</t>
   </si>
   <si>
     <t xml:space="preserve">1,790</t>
@@ -119,10 +119,10 @@
     <t xml:space="preserve">(-1,605; 4,520)</t>
   </si>
   <si>
-    <t xml:space="preserve">-12,310</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(-26,845; 570)</t>
+    <t xml:space="preserve">1,950</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(-825; 4,670)</t>
   </si>
   <si>
     <t xml:space="preserve">990</t>
@@ -146,10 +146,10 @@
     <t xml:space="preserve">(1,175; 6,505)</t>
   </si>
   <si>
-    <t xml:space="preserve">-11,490</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(-21,800; -2,175)</t>
+    <t xml:space="preserve">4,035</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(1,240; 6,670)</t>
   </si>
   <si>
     <t xml:space="preserve">1,905</t>
@@ -173,10 +173,10 @@
     <t xml:space="preserve">(21,690; 27,465)</t>
   </si>
   <si>
-    <t xml:space="preserve">11,965</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(1,835; 21,075)</t>
+    <t xml:space="preserve">25,725</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(22,845; 28,480)</t>
   </si>
   <si>
     <t xml:space="preserve">23,705</t>
@@ -200,10 +200,10 @@
     <t xml:space="preserve">(515; 6,790)</t>
   </si>
   <si>
-    <t xml:space="preserve">-25,935</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(-42,040; -11,745)</t>
+    <t xml:space="preserve">4,600</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(1,895; 7,275)</t>
   </si>
   <si>
     <t xml:space="preserve">(200; 6,540)</t>
@@ -224,10 +224,10 @@
     <t xml:space="preserve">(-865; 3,725)</t>
   </si>
   <si>
-    <t xml:space="preserve">-8,290</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(-15,635; -1,405)</t>
+    <t xml:space="preserve">1,695</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(-505; 3,905)</t>
   </si>
   <si>
     <t xml:space="preserve">(-630; 3,710)</t>
@@ -248,10 +248,10 @@
     <t xml:space="preserve">(-3,835; 1,675)</t>
   </si>
   <si>
-    <t xml:space="preserve">-10,905</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(-19,500; -2,965)</t>
+    <t xml:space="preserve">-180</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(-2,650; 2,250)</t>
   </si>
   <si>
     <t xml:space="preserve">-25</t>
@@ -275,10 +275,10 @@
     <t xml:space="preserve">(-6,315; -185)</t>
   </si>
   <si>
-    <t xml:space="preserve">-32,105</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(-46,645; -18,910)</t>
+    <t xml:space="preserve">-2,980</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(-5,535; -475)</t>
   </si>
   <si>
     <t xml:space="preserve">-2,760</t>
@@ -302,10 +302,10 @@
     <t xml:space="preserve">(-2,950; 3,460)</t>
   </si>
   <si>
-    <t xml:space="preserve">-12,495</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(-21,095; -4,055)</t>
+    <t xml:space="preserve">395</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(-2,200; 2,895)</t>
   </si>
   <si>
     <t xml:space="preserve">600</t>
@@ -329,10 +329,10 @@
     <t xml:space="preserve">(5,575; 11,675)</t>
   </si>
   <si>
-    <t xml:space="preserve">-5,110</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(-13,425; 2,510)</t>
+    <t xml:space="preserve">8,105</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(5,505; 10,630)</t>
   </si>
   <si>
     <t xml:space="preserve">7,360</t>
@@ -356,10 +356,10 @@
     <t xml:space="preserve">(-2,735; 1,220)</t>
   </si>
   <si>
-    <t xml:space="preserve">-9,630</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(-16,685; -3,065)</t>
+    <t xml:space="preserve">-795</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(-2,715; 1,010)</t>
   </si>
   <si>
     <t xml:space="preserve">-925</t>
@@ -386,10 +386,10 @@
     <t xml:space="preserve">(-1,280; 6,290)</t>
   </si>
   <si>
-    <t xml:space="preserve">-1,710</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(-11,930; 7,590)</t>
+    <t xml:space="preserve">290</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(-3,385; 3,790)</t>
   </si>
   <si>
     <t xml:space="preserve">-1,125</t>
@@ -410,10 +410,10 @@
     <t xml:space="preserve">(4,475; 12,495)</t>
   </si>
   <si>
-    <t xml:space="preserve">3,115</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(-7,690; 13,170)</t>
+    <t xml:space="preserve">7,380</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(3,750; 10,945)</t>
   </si>
   <si>
     <t xml:space="preserve">7,060</t>
@@ -437,10 +437,10 @@
     <t xml:space="preserve">(1,045; 9,800)</t>
   </si>
   <si>
-    <t xml:space="preserve">-16,280</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(-34,020; -870)</t>
+    <t xml:space="preserve">6,515</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(2,655; 10,245)</t>
   </si>
   <si>
     <t xml:space="preserve">5,875</t>
@@ -455,19 +455,16 @@
     <t xml:space="preserve">(-7,970; 2,330)</t>
   </si>
   <si>
-    <t xml:space="preserve">-2,980</t>
-  </si>
-  <si>
     <t xml:space="preserve">-2,865</t>
   </si>
   <si>
     <t xml:space="preserve">(-8,140; 2,105)</t>
   </si>
   <si>
-    <t xml:space="preserve">-3,355</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(-14,570; 6,390)</t>
+    <t xml:space="preserve">-2,945</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(-7,240; 1,245)</t>
   </si>
   <si>
     <t xml:space="preserve">-645</t>
@@ -491,10 +488,10 @@
     <t xml:space="preserve">(20,310; 30,885)</t>
   </si>
   <si>
-    <t xml:space="preserve">22,390</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(11,965; 32,040)</t>
+    <t xml:space="preserve">25,735</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(21,420; 29,845)</t>
   </si>
   <si>
     <t xml:space="preserve">27,700</t>
@@ -518,10 +515,7 @@
     <t xml:space="preserve">(1,020; 12,835)</t>
   </si>
   <si>
-    <t xml:space="preserve">-11,745</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(-28,035; 2,690)</t>
+    <t xml:space="preserve">(1,265; 10,350)</t>
   </si>
   <si>
     <t xml:space="preserve">7,395</t>
@@ -542,10 +536,10 @@
     <t xml:space="preserve">(-2,085; 4,910)</t>
   </si>
   <si>
-    <t xml:space="preserve">-11,945</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(-20,990; -3,515)</t>
+    <t xml:space="preserve">1,050</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(-1,825; 3,820)</t>
   </si>
   <si>
     <t xml:space="preserve">880</t>
@@ -569,10 +563,10 @@
     <t xml:space="preserve">(395; 5,515)</t>
   </si>
   <si>
-    <t xml:space="preserve">-8,150</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(-16,645; 70)</t>
+    <t xml:space="preserve">3,325</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(410; 6,220)</t>
   </si>
   <si>
     <t xml:space="preserve">3,135</t>
@@ -596,10 +590,10 @@
     <t xml:space="preserve">(-2,465; 3,605)</t>
   </si>
   <si>
-    <t xml:space="preserve">-41,850</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(-59,685; -25,600)</t>
+    <t xml:space="preserve">-315</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(-3,565; 2,800)</t>
   </si>
   <si>
     <t xml:space="preserve">-800</t>
@@ -623,10 +617,10 @@
     <t xml:space="preserve">(-7,810; -730)</t>
   </si>
   <si>
-    <t xml:space="preserve">-13,045</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(-22,010; -4,515)</t>
+    <t xml:space="preserve">-3,350</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(-6,330; -345)</t>
   </si>
   <si>
     <t xml:space="preserve">-4,380</t>
@@ -650,10 +644,10 @@
     <t xml:space="preserve">(4,960; 11,690)</t>
   </si>
   <si>
-    <t xml:space="preserve">-4,225</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(-12,640; 3,910)</t>
+    <t xml:space="preserve">6,760</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(3,635; 9,910)</t>
   </si>
   <si>
     <t xml:space="preserve">2,600</t>
@@ -692,10 +686,10 @@
     <t xml:space="preserve">(-13,400; 36,025)</t>
   </si>
   <si>
-    <t xml:space="preserve">31,205</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(-6,895; 66,725)</t>
+    <t xml:space="preserve">22,060</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(-900; 44,430)</t>
   </si>
   <si>
     <t xml:space="preserve">20,950</t>
@@ -719,10 +713,10 @@
     <t xml:space="preserve">(214,035; 264,175)</t>
   </si>
   <si>
-    <t xml:space="preserve">265,120</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(220,910; 306,775)</t>
+    <t xml:space="preserve">243,240</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(218,610; 266,700)</t>
   </si>
   <si>
     <t xml:space="preserve">28,835</t>
@@ -740,10 +734,10 @@
     <t xml:space="preserve">(-4,940; 49,265)</t>
   </si>
   <si>
-    <t xml:space="preserve">25,970</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(-52,320; 97,395)</t>
+    <t xml:space="preserve">24,670</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(-165; 48,125)</t>
   </si>
   <si>
     <t xml:space="preserve">45,235</t>
@@ -767,10 +761,10 @@
     <t xml:space="preserve">(10,205; 54,805)</t>
   </si>
   <si>
-    <t xml:space="preserve">-73,990</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(-143,425; -12,155)</t>
+    <t xml:space="preserve">33,355</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(14,275; 51,825)</t>
   </si>
   <si>
     <t xml:space="preserve">30,730</t>
@@ -794,10 +788,10 @@
     <t xml:space="preserve">(-4,495; 27,310)</t>
   </si>
   <si>
-    <t xml:space="preserve">-29,977,380</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(-119,706,000; -8,050)</t>
+    <t xml:space="preserve">28,360</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(7,820; 48,025)</t>
   </si>
   <si>
     <t xml:space="preserve">21,360</t>
@@ -821,10 +815,10 @@
     <t xml:space="preserve">(-48,745; -9,615)</t>
   </si>
   <si>
-    <t xml:space="preserve">-107,725</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(-191,465; -34,400)</t>
+    <t xml:space="preserve">-11,425</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(-33,630; 9,845)</t>
   </si>
   <si>
     <t xml:space="preserve">-27,265</t>
@@ -848,10 +842,10 @@
     <t xml:space="preserve">(-41,320; 1,025)</t>
   </si>
   <si>
-    <t xml:space="preserve">-56,115</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(-117,505; -260)</t>
+    <t xml:space="preserve">-8,505</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(-26,810; 9,205)</t>
   </si>
   <si>
     <t xml:space="preserve">-10,460</t>
@@ -875,10 +869,10 @@
     <t xml:space="preserve">(44,510; 85,625)</t>
   </si>
   <si>
-    <t xml:space="preserve">-11,300</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(-74,995; 45,780)</t>
+    <t xml:space="preserve">65,045</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(47,040; 81,970)</t>
   </si>
   <si>
     <t xml:space="preserve">69,225</t>
@@ -902,10 +896,10 @@
     <t xml:space="preserve">(-3,525; 24,785)</t>
   </si>
   <si>
-    <t xml:space="preserve">-41,955</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(-85,995; -1,680)</t>
+    <t xml:space="preserve">9,350</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(-3,005; 21,775)</t>
   </si>
   <si>
     <t xml:space="preserve">14,245</t>
@@ -1817,25 +1811,25 @@
         <v>146</v>
       </c>
       <c r="E17" t="s">
+        <v>87</v>
+      </c>
+      <c r="F17" t="s">
         <v>147</v>
       </c>
-      <c r="F17" t="s">
+      <c r="G17" t="s">
         <v>148</v>
       </c>
-      <c r="G17" t="s">
+      <c r="H17" t="s">
         <v>149</v>
       </c>
-      <c r="H17" t="s">
+      <c r="I17" t="s">
         <v>150</v>
       </c>
-      <c r="I17" t="s">
+      <c r="J17" t="s">
         <v>151</v>
       </c>
-      <c r="J17" t="s">
+      <c r="K17" t="s">
         <v>152</v>
-      </c>
-      <c r="K17" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="18">
@@ -1846,31 +1840,31 @@
         <v>1918</v>
       </c>
       <c r="C18" t="s">
+        <v>153</v>
+      </c>
+      <c r="D18" t="s">
         <v>154</v>
       </c>
-      <c r="D18" t="s">
+      <c r="E18" t="s">
         <v>155</v>
       </c>
-      <c r="E18" t="s">
+      <c r="F18" t="s">
         <v>156</v>
       </c>
-      <c r="F18" t="s">
+      <c r="G18" t="s">
         <v>157</v>
       </c>
-      <c r="G18" t="s">
+      <c r="H18" t="s">
         <v>158</v>
       </c>
-      <c r="H18" t="s">
+      <c r="I18" t="s">
         <v>159</v>
       </c>
-      <c r="I18" t="s">
+      <c r="J18" t="s">
         <v>160</v>
       </c>
-      <c r="J18" t="s">
+      <c r="K18" t="s">
         <v>161</v>
-      </c>
-      <c r="K18" t="s">
-        <v>162</v>
       </c>
     </row>
     <row r="19">
@@ -1881,31 +1875,31 @@
         <v>1919</v>
       </c>
       <c r="C19" t="s">
+        <v>162</v>
+      </c>
+      <c r="D19" t="s">
         <v>163</v>
       </c>
-      <c r="D19" t="s">
+      <c r="E19" t="s">
         <v>164</v>
       </c>
-      <c r="E19" t="s">
+      <c r="F19" t="s">
         <v>165</v>
       </c>
-      <c r="F19" t="s">
+      <c r="G19" t="s">
         <v>166</v>
       </c>
-      <c r="G19" t="s">
+      <c r="H19" t="s">
+        <v>143</v>
+      </c>
+      <c r="I19" t="s">
         <v>167</v>
       </c>
-      <c r="H19" t="s">
+      <c r="J19" t="s">
         <v>168</v>
       </c>
-      <c r="I19" t="s">
+      <c r="K19" t="s">
         <v>169</v>
-      </c>
-      <c r="J19" t="s">
-        <v>170</v>
-      </c>
-      <c r="K19" t="s">
-        <v>171</v>
       </c>
     </row>
     <row r="20">
@@ -1916,31 +1910,31 @@
         <v>1956</v>
       </c>
       <c r="C20" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="D20" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="E20" t="s">
         <v>33</v>
       </c>
       <c r="F20" t="s">
+        <v>172</v>
+      </c>
+      <c r="G20" t="s">
+        <v>173</v>
+      </c>
+      <c r="H20" t="s">
         <v>174</v>
       </c>
-      <c r="G20" t="s">
+      <c r="I20" t="s">
         <v>175</v>
       </c>
-      <c r="H20" t="s">
+      <c r="J20" t="s">
         <v>176</v>
       </c>
-      <c r="I20" t="s">
+      <c r="K20" t="s">
         <v>177</v>
-      </c>
-      <c r="J20" t="s">
-        <v>178</v>
-      </c>
-      <c r="K20" t="s">
-        <v>179</v>
       </c>
     </row>
     <row r="21">
@@ -1951,31 +1945,31 @@
         <v>1957</v>
       </c>
       <c r="C21" t="s">
+        <v>178</v>
+      </c>
+      <c r="D21" t="s">
+        <v>179</v>
+      </c>
+      <c r="E21" t="s">
         <v>180</v>
       </c>
-      <c r="D21" t="s">
+      <c r="F21" t="s">
         <v>181</v>
       </c>
-      <c r="E21" t="s">
+      <c r="G21" t="s">
         <v>182</v>
       </c>
-      <c r="F21" t="s">
+      <c r="H21" t="s">
         <v>183</v>
       </c>
-      <c r="G21" t="s">
+      <c r="I21" t="s">
         <v>184</v>
       </c>
-      <c r="H21" t="s">
+      <c r="J21" t="s">
         <v>185</v>
       </c>
-      <c r="I21" t="s">
+      <c r="K21" t="s">
         <v>186</v>
-      </c>
-      <c r="J21" t="s">
-        <v>187</v>
-      </c>
-      <c r="K21" t="s">
-        <v>188</v>
       </c>
     </row>
     <row r="22">
@@ -1986,31 +1980,31 @@
         <v>1958</v>
       </c>
       <c r="C22" t="s">
+        <v>187</v>
+      </c>
+      <c r="D22" t="s">
+        <v>188</v>
+      </c>
+      <c r="E22" t="s">
         <v>189</v>
       </c>
-      <c r="D22" t="s">
+      <c r="F22" t="s">
         <v>190</v>
       </c>
-      <c r="E22" t="s">
+      <c r="G22" t="s">
         <v>191</v>
       </c>
-      <c r="F22" t="s">
+      <c r="H22" t="s">
         <v>192</v>
       </c>
-      <c r="G22" t="s">
+      <c r="I22" t="s">
         <v>193</v>
       </c>
-      <c r="H22" t="s">
+      <c r="J22" t="s">
         <v>194</v>
       </c>
-      <c r="I22" t="s">
+      <c r="K22" t="s">
         <v>195</v>
-      </c>
-      <c r="J22" t="s">
-        <v>196</v>
-      </c>
-      <c r="K22" t="s">
-        <v>197</v>
       </c>
     </row>
     <row r="23">
@@ -2021,31 +2015,31 @@
         <v>2019</v>
       </c>
       <c r="C23" t="s">
+        <v>196</v>
+      </c>
+      <c r="D23" t="s">
+        <v>197</v>
+      </c>
+      <c r="E23" t="s">
         <v>198</v>
       </c>
-      <c r="D23" t="s">
+      <c r="F23" t="s">
         <v>199</v>
       </c>
-      <c r="E23" t="s">
+      <c r="G23" t="s">
         <v>200</v>
       </c>
-      <c r="F23" t="s">
+      <c r="H23" t="s">
         <v>201</v>
       </c>
-      <c r="G23" t="s">
+      <c r="I23" t="s">
         <v>202</v>
       </c>
-      <c r="H23" t="s">
+      <c r="J23" t="s">
         <v>203</v>
       </c>
-      <c r="I23" t="s">
+      <c r="K23" t="s">
         <v>204</v>
-      </c>
-      <c r="J23" t="s">
-        <v>205</v>
-      </c>
-      <c r="K23" t="s">
-        <v>206</v>
       </c>
     </row>
     <row r="24">
@@ -2056,31 +2050,31 @@
         <v>2020</v>
       </c>
       <c r="C24" t="s">
+        <v>205</v>
+      </c>
+      <c r="D24" t="s">
+        <v>206</v>
+      </c>
+      <c r="E24" t="s">
         <v>207</v>
       </c>
-      <c r="D24" t="s">
+      <c r="F24" t="s">
         <v>208</v>
       </c>
-      <c r="E24" t="s">
+      <c r="G24" t="s">
         <v>209</v>
       </c>
-      <c r="F24" t="s">
+      <c r="H24" t="s">
         <v>210</v>
       </c>
-      <c r="G24" t="s">
+      <c r="I24" t="s">
         <v>211</v>
       </c>
-      <c r="H24" t="s">
+      <c r="J24" t="s">
         <v>212</v>
       </c>
-      <c r="I24" t="s">
+      <c r="K24" t="s">
         <v>213</v>
-      </c>
-      <c r="J24" t="s">
-        <v>214</v>
-      </c>
-      <c r="K24" t="s">
-        <v>215</v>
       </c>
     </row>
     <row r="25">
@@ -2091,346 +2085,346 @@
         <v>2021</v>
       </c>
       <c r="C25" t="s">
+        <v>214</v>
+      </c>
+      <c r="D25" t="s">
+        <v>214</v>
+      </c>
+      <c r="E25" t="s">
+        <v>215</v>
+      </c>
+      <c r="F25" t="s">
         <v>216</v>
       </c>
-      <c r="D25" t="s">
-        <v>216</v>
-      </c>
-      <c r="E25" t="s">
+      <c r="G25" t="s">
         <v>217</v>
       </c>
-      <c r="F25" t="s">
-        <v>218</v>
-      </c>
-      <c r="G25" t="s">
-        <v>219</v>
-      </c>
       <c r="H25" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="I25" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="J25" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="K25" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="B26" t="n">
         <v>1917</v>
       </c>
       <c r="C26" t="s">
+        <v>219</v>
+      </c>
+      <c r="D26" t="s">
+        <v>220</v>
+      </c>
+      <c r="E26" t="s">
         <v>221</v>
       </c>
-      <c r="D26" t="s">
+      <c r="F26" t="s">
         <v>222</v>
       </c>
-      <c r="E26" t="s">
+      <c r="G26" t="s">
         <v>223</v>
       </c>
-      <c r="F26" t="s">
+      <c r="H26" t="s">
         <v>224</v>
       </c>
-      <c r="G26" t="s">
+      <c r="I26" t="s">
         <v>225</v>
       </c>
-      <c r="H26" t="s">
+      <c r="J26" t="s">
         <v>226</v>
       </c>
-      <c r="I26" t="s">
+      <c r="K26" t="s">
         <v>227</v>
-      </c>
-      <c r="J26" t="s">
-        <v>228</v>
-      </c>
-      <c r="K26" t="s">
-        <v>229</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="B27" t="n">
         <v>1918</v>
       </c>
       <c r="C27" t="s">
+        <v>228</v>
+      </c>
+      <c r="D27" t="s">
+        <v>229</v>
+      </c>
+      <c r="E27" t="s">
         <v>230</v>
       </c>
-      <c r="D27" t="s">
+      <c r="F27" t="s">
         <v>231</v>
       </c>
-      <c r="E27" t="s">
+      <c r="G27" t="s">
         <v>232</v>
       </c>
-      <c r="F27" t="s">
+      <c r="H27" t="s">
         <v>233</v>
       </c>
-      <c r="G27" t="s">
+      <c r="I27" t="s">
         <v>234</v>
       </c>
-      <c r="H27" t="s">
-        <v>235</v>
-      </c>
-      <c r="I27" t="s">
-        <v>236</v>
-      </c>
       <c r="J27" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="K27" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="B28" t="n">
         <v>1919</v>
       </c>
       <c r="C28" t="s">
+        <v>235</v>
+      </c>
+      <c r="D28" t="s">
+        <v>236</v>
+      </c>
+      <c r="E28" t="s">
         <v>237</v>
       </c>
-      <c r="D28" t="s">
+      <c r="F28" t="s">
         <v>238</v>
       </c>
-      <c r="E28" t="s">
+      <c r="G28" t="s">
         <v>239</v>
       </c>
-      <c r="F28" t="s">
+      <c r="H28" t="s">
         <v>240</v>
       </c>
-      <c r="G28" t="s">
+      <c r="I28" t="s">
         <v>241</v>
       </c>
-      <c r="H28" t="s">
+      <c r="J28" t="s">
         <v>242</v>
       </c>
-      <c r="I28" t="s">
+      <c r="K28" t="s">
         <v>243</v>
-      </c>
-      <c r="J28" t="s">
-        <v>244</v>
-      </c>
-      <c r="K28" t="s">
-        <v>245</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="B29" t="n">
         <v>1956</v>
       </c>
       <c r="C29" t="s">
+        <v>244</v>
+      </c>
+      <c r="D29" t="s">
+        <v>245</v>
+      </c>
+      <c r="E29" t="s">
         <v>246</v>
       </c>
-      <c r="D29" t="s">
+      <c r="F29" t="s">
         <v>247</v>
       </c>
-      <c r="E29" t="s">
+      <c r="G29" t="s">
         <v>248</v>
       </c>
-      <c r="F29" t="s">
+      <c r="H29" t="s">
         <v>249</v>
       </c>
-      <c r="G29" t="s">
+      <c r="I29" t="s">
         <v>250</v>
       </c>
-      <c r="H29" t="s">
+      <c r="J29" t="s">
         <v>251</v>
       </c>
-      <c r="I29" t="s">
+      <c r="K29" t="s">
         <v>252</v>
-      </c>
-      <c r="J29" t="s">
-        <v>253</v>
-      </c>
-      <c r="K29" t="s">
-        <v>254</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="B30" t="n">
         <v>1957</v>
       </c>
       <c r="C30" t="s">
+        <v>253</v>
+      </c>
+      <c r="D30" t="s">
+        <v>254</v>
+      </c>
+      <c r="E30" t="s">
         <v>255</v>
       </c>
-      <c r="D30" t="s">
+      <c r="F30" t="s">
         <v>256</v>
       </c>
-      <c r="E30" t="s">
+      <c r="G30" t="s">
         <v>257</v>
       </c>
-      <c r="F30" t="s">
+      <c r="H30" t="s">
         <v>258</v>
       </c>
-      <c r="G30" t="s">
+      <c r="I30" t="s">
         <v>259</v>
       </c>
-      <c r="H30" t="s">
+      <c r="J30" t="s">
         <v>260</v>
       </c>
-      <c r="I30" t="s">
+      <c r="K30" t="s">
         <v>261</v>
-      </c>
-      <c r="J30" t="s">
-        <v>262</v>
-      </c>
-      <c r="K30" t="s">
-        <v>263</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="B31" t="n">
         <v>1958</v>
       </c>
       <c r="C31" t="s">
+        <v>262</v>
+      </c>
+      <c r="D31" t="s">
+        <v>263</v>
+      </c>
+      <c r="E31" t="s">
         <v>264</v>
       </c>
-      <c r="D31" t="s">
+      <c r="F31" t="s">
         <v>265</v>
       </c>
-      <c r="E31" t="s">
+      <c r="G31" t="s">
         <v>266</v>
       </c>
-      <c r="F31" t="s">
+      <c r="H31" t="s">
         <v>267</v>
       </c>
-      <c r="G31" t="s">
+      <c r="I31" t="s">
         <v>268</v>
       </c>
-      <c r="H31" t="s">
+      <c r="J31" t="s">
         <v>269</v>
       </c>
-      <c r="I31" t="s">
+      <c r="K31" t="s">
         <v>270</v>
-      </c>
-      <c r="J31" t="s">
-        <v>271</v>
-      </c>
-      <c r="K31" t="s">
-        <v>272</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="B32" t="n">
         <v>2019</v>
       </c>
       <c r="C32" t="s">
+        <v>271</v>
+      </c>
+      <c r="D32" t="s">
+        <v>272</v>
+      </c>
+      <c r="E32" t="s">
         <v>273</v>
       </c>
-      <c r="D32" t="s">
+      <c r="F32" t="s">
         <v>274</v>
       </c>
-      <c r="E32" t="s">
+      <c r="G32" t="s">
         <v>275</v>
       </c>
-      <c r="F32" t="s">
+      <c r="H32" t="s">
         <v>276</v>
       </c>
-      <c r="G32" t="s">
+      <c r="I32" t="s">
         <v>277</v>
       </c>
-      <c r="H32" t="s">
+      <c r="J32" t="s">
         <v>278</v>
       </c>
-      <c r="I32" t="s">
+      <c r="K32" t="s">
         <v>279</v>
-      </c>
-      <c r="J32" t="s">
-        <v>280</v>
-      </c>
-      <c r="K32" t="s">
-        <v>281</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="B33" t="n">
         <v>2020</v>
       </c>
       <c r="C33" t="s">
+        <v>280</v>
+      </c>
+      <c r="D33" t="s">
+        <v>281</v>
+      </c>
+      <c r="E33" t="s">
         <v>282</v>
       </c>
-      <c r="D33" t="s">
+      <c r="F33" t="s">
         <v>283</v>
       </c>
-      <c r="E33" t="s">
+      <c r="G33" t="s">
         <v>284</v>
       </c>
-      <c r="F33" t="s">
+      <c r="H33" t="s">
         <v>285</v>
       </c>
-      <c r="G33" t="s">
+      <c r="I33" t="s">
         <v>286</v>
       </c>
-      <c r="H33" t="s">
+      <c r="J33" t="s">
         <v>287</v>
       </c>
-      <c r="I33" t="s">
+      <c r="K33" t="s">
         <v>288</v>
-      </c>
-      <c r="J33" t="s">
-        <v>289</v>
-      </c>
-      <c r="K33" t="s">
-        <v>290</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="B34" t="n">
         <v>2021</v>
       </c>
       <c r="C34" t="s">
+        <v>289</v>
+      </c>
+      <c r="D34" t="s">
+        <v>290</v>
+      </c>
+      <c r="E34" t="s">
         <v>291</v>
       </c>
-      <c r="D34" t="s">
+      <c r="F34" t="s">
         <v>292</v>
       </c>
-      <c r="E34" t="s">
+      <c r="G34" t="s">
         <v>293</v>
       </c>
-      <c r="F34" t="s">
+      <c r="H34" t="s">
         <v>294</v>
       </c>
-      <c r="G34" t="s">
+      <c r="I34" t="s">
         <v>295</v>
       </c>
-      <c r="H34" t="s">
+      <c r="J34" t="s">
         <v>296</v>
       </c>
-      <c r="I34" t="s">
+      <c r="K34" t="s">
         <v>297</v>
-      </c>
-      <c r="J34" t="s">
-        <v>298</v>
-      </c>
-      <c r="K34" t="s">
-        <v>299</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
tabsets for figs & small formating updates
</commit_message>
<xml_diff>
--- a/paper/Table_S1.xlsx
+++ b/paper/Table_S1.xlsx
@@ -53,7 +53,7 @@
     <t xml:space="preserve">1,380</t>
   </si>
   <si>
-    <t xml:space="preserve">(-1,550; 4,255)</t>
+    <t xml:space="preserve">(-1,550 to 4,255)</t>
   </si>
   <si>
     <t xml:space="preserve">1,100</t>
@@ -62,25 +62,25 @@
     <t xml:space="preserve">1,300</t>
   </si>
   <si>
-    <t xml:space="preserve">(-1,650; 4,130)</t>
+    <t xml:space="preserve">(-1,650 to 4,130)</t>
   </si>
   <si>
     <t xml:space="preserve">1,680</t>
   </si>
   <si>
-    <t xml:space="preserve">(-865; 4,190)</t>
+    <t xml:space="preserve">(-865 to 4,190)</t>
   </si>
   <si>
     <t xml:space="preserve">-410</t>
   </si>
   <si>
-    <t xml:space="preserve">(-3,405; 2,510)</t>
+    <t xml:space="preserve">(-3,405 to 2,510)</t>
   </si>
   <si>
     <t xml:space="preserve">3,455</t>
   </si>
   <si>
-    <t xml:space="preserve">(705; 6,120)</t>
+    <t xml:space="preserve">(705 to 6,120)</t>
   </si>
   <si>
     <t xml:space="preserve">3,380</t>
@@ -89,25 +89,25 @@
     <t xml:space="preserve">3,360</t>
   </si>
   <si>
-    <t xml:space="preserve">(605; 6,015)</t>
+    <t xml:space="preserve">(605 to 6,015)</t>
   </si>
   <si>
     <t xml:space="preserve">2,395</t>
   </si>
   <si>
-    <t xml:space="preserve">(-310; 5,020)</t>
+    <t xml:space="preserve">(-310 to 5,020)</t>
   </si>
   <si>
     <t xml:space="preserve">1,790</t>
   </si>
   <si>
-    <t xml:space="preserve">(-1,110; 4,565)</t>
+    <t xml:space="preserve">(-1,110 to 4,565)</t>
   </si>
   <si>
     <t xml:space="preserve">1,920</t>
   </si>
   <si>
-    <t xml:space="preserve">(-1,265; 5,010)</t>
+    <t xml:space="preserve">(-1,265 to 5,010)</t>
   </si>
   <si>
     <t xml:space="preserve">1,975</t>
@@ -116,25 +116,25 @@
     <t xml:space="preserve">1,585</t>
   </si>
   <si>
-    <t xml:space="preserve">(-1,605; 4,520)</t>
+    <t xml:space="preserve">(-1,605 to 4,520)</t>
   </si>
   <si>
     <t xml:space="preserve">1,950</t>
   </si>
   <si>
-    <t xml:space="preserve">(-825; 4,670)</t>
+    <t xml:space="preserve">(-825 to 4,670)</t>
   </si>
   <si>
     <t xml:space="preserve">990</t>
   </si>
   <si>
-    <t xml:space="preserve">(-2,140; 4,045)</t>
+    <t xml:space="preserve">(-2,140 to 4,045)</t>
   </si>
   <si>
     <t xml:space="preserve">3,810</t>
   </si>
   <si>
-    <t xml:space="preserve">(1,155; 6,395)</t>
+    <t xml:space="preserve">(1,155 to 6,395)</t>
   </si>
   <si>
     <t xml:space="preserve">3,630</t>
@@ -143,25 +143,25 @@
     <t xml:space="preserve">3,855</t>
   </si>
   <si>
-    <t xml:space="preserve">(1,175; 6,505)</t>
+    <t xml:space="preserve">(1,175 to 6,505)</t>
   </si>
   <si>
     <t xml:space="preserve">4,035</t>
   </si>
   <si>
-    <t xml:space="preserve">(1,240; 6,670)</t>
+    <t xml:space="preserve">(1,240 to 6,670)</t>
   </si>
   <si>
     <t xml:space="preserve">1,905</t>
   </si>
   <si>
-    <t xml:space="preserve">(-925; 4,630)</t>
+    <t xml:space="preserve">(-925 to 4,630)</t>
   </si>
   <si>
     <t xml:space="preserve">24,730</t>
   </si>
   <si>
-    <t xml:space="preserve">(21,925; 27,455)</t>
+    <t xml:space="preserve">(21,925 to 27,455)</t>
   </si>
   <si>
     <t xml:space="preserve">24,460</t>
@@ -170,25 +170,25 @@
     <t xml:space="preserve">24,625</t>
   </si>
   <si>
-    <t xml:space="preserve">(21,690; 27,465)</t>
+    <t xml:space="preserve">(21,690 to 27,465)</t>
   </si>
   <si>
     <t xml:space="preserve">25,725</t>
   </si>
   <si>
-    <t xml:space="preserve">(22,845; 28,480)</t>
+    <t xml:space="preserve">(22,845 to 28,480)</t>
   </si>
   <si>
     <t xml:space="preserve">23,705</t>
   </si>
   <si>
-    <t xml:space="preserve">(20,540; 26,705)</t>
+    <t xml:space="preserve">(20,540 to 26,705)</t>
   </si>
   <si>
     <t xml:space="preserve">3,730</t>
   </si>
   <si>
-    <t xml:space="preserve">(510; 6,835)</t>
+    <t xml:space="preserve">(510 to 6,835)</t>
   </si>
   <si>
     <t xml:space="preserve">3,820</t>
@@ -197,22 +197,22 @@
     <t xml:space="preserve">3,700</t>
   </si>
   <si>
-    <t xml:space="preserve">(515; 6,790)</t>
+    <t xml:space="preserve">(515 to 6,790)</t>
   </si>
   <si>
     <t xml:space="preserve">4,600</t>
   </si>
   <si>
-    <t xml:space="preserve">(1,895; 7,275)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(200; 6,540)</t>
+    <t xml:space="preserve">(1,895 to 7,275)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(200 to 6,540)</t>
   </si>
   <si>
     <t xml:space="preserve">1,535</t>
   </si>
   <si>
-    <t xml:space="preserve">(-775; 3,750)</t>
+    <t xml:space="preserve">(-775 to 3,750)</t>
   </si>
   <si>
     <t xml:space="preserve">1,555</t>
@@ -221,22 +221,22 @@
     <t xml:space="preserve">1,470</t>
   </si>
   <si>
-    <t xml:space="preserve">(-865; 3,725)</t>
+    <t xml:space="preserve">(-865 to 3,725)</t>
   </si>
   <si>
     <t xml:space="preserve">1,695</t>
   </si>
   <si>
-    <t xml:space="preserve">(-505; 3,905)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(-630; 3,710)</t>
+    <t xml:space="preserve">(-505 to 3,905)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(-630 to 3,710)</t>
   </si>
   <si>
     <t xml:space="preserve">-920</t>
   </si>
   <si>
-    <t xml:space="preserve">(-3,680; 1,805)</t>
+    <t xml:space="preserve">(-3,680 to 1,805)</t>
   </si>
   <si>
     <t xml:space="preserve">-1,200</t>
@@ -245,25 +245,25 @@
     <t xml:space="preserve">-1,035</t>
   </si>
   <si>
-    <t xml:space="preserve">(-3,835; 1,675)</t>
+    <t xml:space="preserve">(-3,835 to 1,675)</t>
   </si>
   <si>
     <t xml:space="preserve">-180</t>
   </si>
   <si>
-    <t xml:space="preserve">(-2,650; 2,250)</t>
+    <t xml:space="preserve">(-2,650 to 2,250)</t>
   </si>
   <si>
     <t xml:space="preserve">-25</t>
   </si>
   <si>
-    <t xml:space="preserve">(-2,440; 2,295)</t>
+    <t xml:space="preserve">(-2,440 to 2,295)</t>
   </si>
   <si>
     <t xml:space="preserve">-3,705</t>
   </si>
   <si>
-    <t xml:space="preserve">(-6,950; -605)</t>
+    <t xml:space="preserve">(-6,950 to -605)</t>
   </si>
   <si>
     <t xml:space="preserve">-3,360</t>
@@ -272,25 +272,25 @@
     <t xml:space="preserve">-3,190</t>
   </si>
   <si>
-    <t xml:space="preserve">(-6,315; -185)</t>
+    <t xml:space="preserve">(-6,315 to -185)</t>
   </si>
   <si>
     <t xml:space="preserve">-2,980</t>
   </si>
   <si>
-    <t xml:space="preserve">(-5,535; -475)</t>
+    <t xml:space="preserve">(-5,535 to -475)</t>
   </si>
   <si>
     <t xml:space="preserve">-2,760</t>
   </si>
   <si>
-    <t xml:space="preserve">(-5,095; -380)</t>
+    <t xml:space="preserve">(-5,095 to -380)</t>
   </si>
   <si>
     <t xml:space="preserve">165</t>
   </si>
   <si>
-    <t xml:space="preserve">(-3,210; 3,400)</t>
+    <t xml:space="preserve">(-3,210 to 3,400)</t>
   </si>
   <si>
     <t xml:space="preserve">280</t>
@@ -299,25 +299,25 @@
     <t xml:space="preserve">320</t>
   </si>
   <si>
-    <t xml:space="preserve">(-2,950; 3,460)</t>
+    <t xml:space="preserve">(-2,950 to 3,460)</t>
   </si>
   <si>
     <t xml:space="preserve">395</t>
   </si>
   <si>
-    <t xml:space="preserve">(-2,200; 2,895)</t>
+    <t xml:space="preserve">(-2,200 to 2,895)</t>
   </si>
   <si>
     <t xml:space="preserve">600</t>
   </si>
   <si>
-    <t xml:space="preserve">(-1,865; 2,975)</t>
+    <t xml:space="preserve">(-1,865 to 2,975)</t>
   </si>
   <si>
     <t xml:space="preserve">8,430</t>
   </si>
   <si>
-    <t xml:space="preserve">(5,255; 11,450)</t>
+    <t xml:space="preserve">(5,255 to 11,450)</t>
   </si>
   <si>
     <t xml:space="preserve">8,810</t>
@@ -326,25 +326,25 @@
     <t xml:space="preserve">8,685</t>
   </si>
   <si>
-    <t xml:space="preserve">(5,575; 11,675)</t>
+    <t xml:space="preserve">(5,575 to 11,675)</t>
   </si>
   <si>
     <t xml:space="preserve">8,105</t>
   </si>
   <si>
-    <t xml:space="preserve">(5,505; 10,630)</t>
+    <t xml:space="preserve">(5,505 to 10,630)</t>
   </si>
   <si>
     <t xml:space="preserve">7,360</t>
   </si>
   <si>
-    <t xml:space="preserve">(4,395; 10,240)</t>
+    <t xml:space="preserve">(4,395 to 10,240)</t>
   </si>
   <si>
     <t xml:space="preserve">-1,000</t>
   </si>
   <si>
-    <t xml:space="preserve">(-3,085; 955)</t>
+    <t xml:space="preserve">(-3,085 to 955)</t>
   </si>
   <si>
     <t xml:space="preserve">-845</t>
@@ -353,19 +353,19 @@
     <t xml:space="preserve">-715</t>
   </si>
   <si>
-    <t xml:space="preserve">(-2,735; 1,220)</t>
+    <t xml:space="preserve">(-2,735 to 1,220)</t>
   </si>
   <si>
     <t xml:space="preserve">-795</t>
   </si>
   <si>
-    <t xml:space="preserve">(-2,715; 1,010)</t>
+    <t xml:space="preserve">(-2,715 to 1,010)</t>
   </si>
   <si>
     <t xml:space="preserve">-925</t>
   </si>
   <si>
-    <t xml:space="preserve">(-3,280; 1,375)</t>
+    <t xml:space="preserve">(-3,280 to 1,375)</t>
   </si>
   <si>
     <t xml:space="preserve">Sweden</t>
@@ -374,7 +374,7 @@
     <t xml:space="preserve">2,495</t>
   </si>
   <si>
-    <t xml:space="preserve">(-1,400; 6,155)</t>
+    <t xml:space="preserve">(-1,400 to 6,155)</t>
   </si>
   <si>
     <t xml:space="preserve">2,785</t>
@@ -383,22 +383,22 @@
     <t xml:space="preserve">2,540</t>
   </si>
   <si>
-    <t xml:space="preserve">(-1,280; 6,290)</t>
+    <t xml:space="preserve">(-1,280 to 6,290)</t>
   </si>
   <si>
     <t xml:space="preserve">290</t>
   </si>
   <si>
-    <t xml:space="preserve">(-3,385; 3,790)</t>
+    <t xml:space="preserve">(-3,385 to 3,790)</t>
   </si>
   <si>
     <t xml:space="preserve">-1,125</t>
   </si>
   <si>
-    <t xml:space="preserve">(-5,425; 2,960)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(4,870; 12,575)</t>
+    <t xml:space="preserve">(-5,425 to 2,960)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(4,870 to 12,575)</t>
   </si>
   <si>
     <t xml:space="preserve">8,720</t>
@@ -407,25 +407,25 @@
     <t xml:space="preserve">8,525</t>
   </si>
   <si>
-    <t xml:space="preserve">(4,475; 12,495)</t>
+    <t xml:space="preserve">(4,475 to 12,495)</t>
   </si>
   <si>
     <t xml:space="preserve">7,380</t>
   </si>
   <si>
-    <t xml:space="preserve">(3,750; 10,945)</t>
+    <t xml:space="preserve">(3,750 to 10,945)</t>
   </si>
   <si>
     <t xml:space="preserve">7,060</t>
   </si>
   <si>
-    <t xml:space="preserve">(2,930; 11,055)</t>
+    <t xml:space="preserve">(2,930 to 11,055)</t>
   </si>
   <si>
     <t xml:space="preserve">5,295</t>
   </si>
   <si>
-    <t xml:space="preserve">(800; 9,480)</t>
+    <t xml:space="preserve">(800 to 9,480)</t>
   </si>
   <si>
     <t xml:space="preserve">6,365</t>
@@ -434,49 +434,49 @@
     <t xml:space="preserve">5,570</t>
   </si>
   <si>
-    <t xml:space="preserve">(1,045; 9,800)</t>
+    <t xml:space="preserve">(1,045 to 9,800)</t>
   </si>
   <si>
     <t xml:space="preserve">6,515</t>
   </si>
   <si>
-    <t xml:space="preserve">(2,655; 10,245)</t>
+    <t xml:space="preserve">(2,655 to 10,245)</t>
   </si>
   <si>
     <t xml:space="preserve">5,875</t>
   </si>
   <si>
-    <t xml:space="preserve">(1,405; 10,255)</t>
+    <t xml:space="preserve">(1,405 to 10,255)</t>
   </si>
   <si>
     <t xml:space="preserve">-2,640</t>
   </si>
   <si>
-    <t xml:space="preserve">(-7,970; 2,330)</t>
+    <t xml:space="preserve">(-7,970 to 2,330)</t>
   </si>
   <si>
     <t xml:space="preserve">-2,865</t>
   </si>
   <si>
-    <t xml:space="preserve">(-8,140; 2,105)</t>
+    <t xml:space="preserve">(-8,140 to 2,105)</t>
   </si>
   <si>
     <t xml:space="preserve">-2,945</t>
   </si>
   <si>
-    <t xml:space="preserve">(-7,240; 1,245)</t>
+    <t xml:space="preserve">(-7,240 to 1,245)</t>
   </si>
   <si>
     <t xml:space="preserve">-645</t>
   </si>
   <si>
-    <t xml:space="preserve">(-4,165; 2,725)</t>
+    <t xml:space="preserve">(-4,165 to 2,725)</t>
   </si>
   <si>
     <t xml:space="preserve">25,935</t>
   </si>
   <si>
-    <t xml:space="preserve">(20,595; 31,085)</t>
+    <t xml:space="preserve">(20,595 to 31,085)</t>
   </si>
   <si>
     <t xml:space="preserve">25,505</t>
@@ -485,25 +485,25 @@
     <t xml:space="preserve">25,695</t>
   </si>
   <si>
-    <t xml:space="preserve">(20,310; 30,885)</t>
+    <t xml:space="preserve">(20,310 to 30,885)</t>
   </si>
   <si>
     <t xml:space="preserve">25,735</t>
   </si>
   <si>
-    <t xml:space="preserve">(21,420; 29,845)</t>
+    <t xml:space="preserve">(21,420 to 29,845)</t>
   </si>
   <si>
     <t xml:space="preserve">27,700</t>
   </si>
   <si>
-    <t xml:space="preserve">(23,945; 31,250)</t>
+    <t xml:space="preserve">(23,945 to 31,250)</t>
   </si>
   <si>
     <t xml:space="preserve">7,245</t>
   </si>
   <si>
-    <t xml:space="preserve">(1,180; 12,965)</t>
+    <t xml:space="preserve">(1,180 to 12,965)</t>
   </si>
   <si>
     <t xml:space="preserve">8,260</t>
@@ -512,46 +512,46 @@
     <t xml:space="preserve">7,140</t>
   </si>
   <si>
-    <t xml:space="preserve">(1,020; 12,835)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(1,265; 10,350)</t>
+    <t xml:space="preserve">(1,020 to 12,835)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(1,265 to 10,350)</t>
   </si>
   <si>
     <t xml:space="preserve">7,395</t>
   </si>
   <si>
-    <t xml:space="preserve">(3,625; 11,080)</t>
+    <t xml:space="preserve">(3,625 to 11,080)</t>
   </si>
   <si>
     <t xml:space="preserve">1,080</t>
   </si>
   <si>
-    <t xml:space="preserve">(-2,395; 4,445)</t>
+    <t xml:space="preserve">(-2,395 to 4,445)</t>
   </si>
   <si>
     <t xml:space="preserve">1,450</t>
   </si>
   <si>
-    <t xml:space="preserve">(-2,085; 4,910)</t>
+    <t xml:space="preserve">(-2,085 to 4,910)</t>
   </si>
   <si>
     <t xml:space="preserve">1,050</t>
   </si>
   <si>
-    <t xml:space="preserve">(-1,825; 3,820)</t>
+    <t xml:space="preserve">(-1,825 to 3,820)</t>
   </si>
   <si>
     <t xml:space="preserve">880</t>
   </si>
   <si>
-    <t xml:space="preserve">(-2,410; 4,065)</t>
+    <t xml:space="preserve">(-2,410 to 4,065)</t>
   </si>
   <si>
     <t xml:space="preserve">2,760</t>
   </si>
   <si>
-    <t xml:space="preserve">(100; 5,340)</t>
+    <t xml:space="preserve">(100 to 5,340)</t>
   </si>
   <si>
     <t xml:space="preserve">3,040</t>
@@ -560,25 +560,25 @@
     <t xml:space="preserve">2,990</t>
   </si>
   <si>
-    <t xml:space="preserve">(395; 5,515)</t>
+    <t xml:space="preserve">(395 to 5,515)</t>
   </si>
   <si>
     <t xml:space="preserve">3,325</t>
   </si>
   <si>
-    <t xml:space="preserve">(410; 6,220)</t>
+    <t xml:space="preserve">(410 to 6,220)</t>
   </si>
   <si>
     <t xml:space="preserve">3,135</t>
   </si>
   <si>
-    <t xml:space="preserve">(-470; 6,575)</t>
+    <t xml:space="preserve">(-470 to 6,575)</t>
   </si>
   <si>
     <t xml:space="preserve">-360</t>
   </si>
   <si>
-    <t xml:space="preserve">(-3,505; 2,720)</t>
+    <t xml:space="preserve">(-3,505 to 2,720)</t>
   </si>
   <si>
     <t xml:space="preserve">1,040</t>
@@ -587,25 +587,25 @@
     <t xml:space="preserve">620</t>
   </si>
   <si>
-    <t xml:space="preserve">(-2,465; 3,605)</t>
+    <t xml:space="preserve">(-2,465 to 3,605)</t>
   </si>
   <si>
     <t xml:space="preserve">-315</t>
   </si>
   <si>
-    <t xml:space="preserve">(-3,565; 2,800)</t>
+    <t xml:space="preserve">(-3,565 to 2,800)</t>
   </si>
   <si>
     <t xml:space="preserve">-800</t>
   </si>
   <si>
-    <t xml:space="preserve">(-4,875; 3,060)</t>
+    <t xml:space="preserve">(-4,875 to 3,060)</t>
   </si>
   <si>
     <t xml:space="preserve">-4,365</t>
   </si>
   <si>
-    <t xml:space="preserve">(-8,015; -795)</t>
+    <t xml:space="preserve">(-8,015 to -795)</t>
   </si>
   <si>
     <t xml:space="preserve">-4,390</t>
@@ -614,25 +614,25 @@
     <t xml:space="preserve">-4,255</t>
   </si>
   <si>
-    <t xml:space="preserve">(-7,810; -730)</t>
+    <t xml:space="preserve">(-7,810 to -730)</t>
   </si>
   <si>
     <t xml:space="preserve">-3,350</t>
   </si>
   <si>
-    <t xml:space="preserve">(-6,330; -345)</t>
+    <t xml:space="preserve">(-6,330 to -345)</t>
   </si>
   <si>
     <t xml:space="preserve">-4,380</t>
   </si>
   <si>
-    <t xml:space="preserve">(-7,125; -1,695)</t>
+    <t xml:space="preserve">(-7,125 to -1,695)</t>
   </si>
   <si>
     <t xml:space="preserve">7,655</t>
   </si>
   <si>
-    <t xml:space="preserve">(4,200; 10,985)</t>
+    <t xml:space="preserve">(4,200 to 10,985)</t>
   </si>
   <si>
     <t xml:space="preserve">8,465</t>
@@ -641,19 +641,19 @@
     <t xml:space="preserve">8,405</t>
   </si>
   <si>
-    <t xml:space="preserve">(4,960; 11,690)</t>
+    <t xml:space="preserve">(4,960 to 11,690)</t>
   </si>
   <si>
     <t xml:space="preserve">6,760</t>
   </si>
   <si>
-    <t xml:space="preserve">(3,635; 9,910)</t>
+    <t xml:space="preserve">(3,635 to 9,910)</t>
   </si>
   <si>
     <t xml:space="preserve">2,600</t>
   </si>
   <si>
-    <t xml:space="preserve">(-690; 5,750)</t>
+    <t xml:space="preserve">(-690 to 5,750)</t>
   </si>
   <si>
     <t xml:space="preserve">--</t>
@@ -665,7 +665,7 @@
     <t xml:space="preserve">750</t>
   </si>
   <si>
-    <t xml:space="preserve">(-1,845; 3,160)</t>
+    <t xml:space="preserve">(-1,845 to 3,160)</t>
   </si>
   <si>
     <t xml:space="preserve">Spain</t>
@@ -674,7 +674,7 @@
     <t xml:space="preserve">11,645</t>
   </si>
   <si>
-    <t xml:space="preserve">(-13,875; 36,180)</t>
+    <t xml:space="preserve">(-13,875 to 36,180)</t>
   </si>
   <si>
     <t xml:space="preserve">12,155</t>
@@ -683,25 +683,25 @@
     <t xml:space="preserve">12,020</t>
   </si>
   <si>
-    <t xml:space="preserve">(-13,400; 36,025)</t>
+    <t xml:space="preserve">(-13,400 to 36,025)</t>
   </si>
   <si>
     <t xml:space="preserve">22,060</t>
   </si>
   <si>
-    <t xml:space="preserve">(-900; 44,430)</t>
+    <t xml:space="preserve">(-900 to 44,430)</t>
   </si>
   <si>
     <t xml:space="preserve">20,950</t>
   </si>
   <si>
-    <t xml:space="preserve">(1,005; 40,565)</t>
+    <t xml:space="preserve">(1,005 to 40,565)</t>
   </si>
   <si>
     <t xml:space="preserve">241,660</t>
   </si>
   <si>
-    <t xml:space="preserve">(215,790; 266,105)</t>
+    <t xml:space="preserve">(215,790 to 266,105)</t>
   </si>
   <si>
     <t xml:space="preserve">239,680</t>
@@ -710,19 +710,19 @@
     <t xml:space="preserve">239,495</t>
   </si>
   <si>
-    <t xml:space="preserve">(214,035; 264,175)</t>
+    <t xml:space="preserve">(214,035 to 264,175)</t>
   </si>
   <si>
     <t xml:space="preserve">243,240</t>
   </si>
   <si>
-    <t xml:space="preserve">(218,610; 266,700)</t>
+    <t xml:space="preserve">(218,610 to 266,700)</t>
   </si>
   <si>
     <t xml:space="preserve">28,835</t>
   </si>
   <si>
-    <t xml:space="preserve">(1,100; 55,560)</t>
+    <t xml:space="preserve">(1,100 to 55,560)</t>
   </si>
   <si>
     <t xml:space="preserve">23,340</t>
@@ -731,25 +731,25 @@
     <t xml:space="preserve">22,835</t>
   </si>
   <si>
-    <t xml:space="preserve">(-4,940; 49,265)</t>
+    <t xml:space="preserve">(-4,940 to 49,265)</t>
   </si>
   <si>
     <t xml:space="preserve">24,670</t>
   </si>
   <si>
-    <t xml:space="preserve">(-165; 48,125)</t>
+    <t xml:space="preserve">(-165 to 48,125)</t>
   </si>
   <si>
     <t xml:space="preserve">45,235</t>
   </si>
   <si>
-    <t xml:space="preserve">(21,520; 67,910)</t>
+    <t xml:space="preserve">(21,520 to 67,910)</t>
   </si>
   <si>
     <t xml:space="preserve">32,305</t>
   </si>
   <si>
-    <t xml:space="preserve">(9,145; 53,685)</t>
+    <t xml:space="preserve">(9,145 to 53,685)</t>
   </si>
   <si>
     <t xml:space="preserve">39,455</t>
@@ -758,25 +758,25 @@
     <t xml:space="preserve">33,085</t>
   </si>
   <si>
-    <t xml:space="preserve">(10,205; 54,805)</t>
+    <t xml:space="preserve">(10,205 to 54,805)</t>
   </si>
   <si>
     <t xml:space="preserve">33,355</t>
   </si>
   <si>
-    <t xml:space="preserve">(14,275; 51,825)</t>
+    <t xml:space="preserve">(14,275 to 51,825)</t>
   </si>
   <si>
     <t xml:space="preserve">30,730</t>
   </si>
   <si>
-    <t xml:space="preserve">(15,545; 45,480)</t>
+    <t xml:space="preserve">(15,545 to 45,480)</t>
   </si>
   <si>
     <t xml:space="preserve">13,225</t>
   </si>
   <si>
-    <t xml:space="preserve">(-2,660; 28,785)</t>
+    <t xml:space="preserve">(-2,660 to 28,785)</t>
   </si>
   <si>
     <t xml:space="preserve">10,715</t>
@@ -785,25 +785,25 @@
     <t xml:space="preserve">11,675</t>
   </si>
   <si>
-    <t xml:space="preserve">(-4,495; 27,310)</t>
+    <t xml:space="preserve">(-4,495 to 27,310)</t>
   </si>
   <si>
     <t xml:space="preserve">28,360</t>
   </si>
   <si>
-    <t xml:space="preserve">(7,820; 48,025)</t>
+    <t xml:space="preserve">(7,820 to 48,025)</t>
   </si>
   <si>
     <t xml:space="preserve">21,360</t>
   </si>
   <si>
-    <t xml:space="preserve">(4,365; 37,570)</t>
+    <t xml:space="preserve">(4,365 to 37,570)</t>
   </si>
   <si>
     <t xml:space="preserve">-28,160</t>
   </si>
   <si>
-    <t xml:space="preserve">(-47,480; -9,435)</t>
+    <t xml:space="preserve">(-47,480 to -9,435)</t>
   </si>
   <si>
     <t xml:space="preserve">-32,630</t>
@@ -812,25 +812,25 @@
     <t xml:space="preserve">-28,615</t>
   </si>
   <si>
-    <t xml:space="preserve">(-48,745; -9,615)</t>
+    <t xml:space="preserve">(-48,745 to -9,615)</t>
   </si>
   <si>
     <t xml:space="preserve">-11,425</t>
   </si>
   <si>
-    <t xml:space="preserve">(-33,630; 9,845)</t>
+    <t xml:space="preserve">(-33,630 to 9,845)</t>
   </si>
   <si>
     <t xml:space="preserve">-27,265</t>
   </si>
   <si>
-    <t xml:space="preserve">(-44,020; -10,910)</t>
+    <t xml:space="preserve">(-44,020 to -10,910)</t>
   </si>
   <si>
     <t xml:space="preserve">-13,370</t>
   </si>
   <si>
-    <t xml:space="preserve">(-34,800; 7,185)</t>
+    <t xml:space="preserve">(-34,800 to 7,185)</t>
   </si>
   <si>
     <t xml:space="preserve">-20,505</t>
@@ -839,25 +839,25 @@
     <t xml:space="preserve">-19,885</t>
   </si>
   <si>
-    <t xml:space="preserve">(-41,320; 1,025)</t>
+    <t xml:space="preserve">(-41,320 to 1,025)</t>
   </si>
   <si>
     <t xml:space="preserve">-8,505</t>
   </si>
   <si>
-    <t xml:space="preserve">(-26,810; 9,205)</t>
+    <t xml:space="preserve">(-26,810 to 9,205)</t>
   </si>
   <si>
     <t xml:space="preserve">-10,460</t>
   </si>
   <si>
-    <t xml:space="preserve">(-31,415; 9,695)</t>
+    <t xml:space="preserve">(-31,415 to 9,695)</t>
   </si>
   <si>
     <t xml:space="preserve">72,330</t>
   </si>
   <si>
-    <t xml:space="preserve">(51,940; 92,410)</t>
+    <t xml:space="preserve">(51,940 to 92,410)</t>
   </si>
   <si>
     <t xml:space="preserve">65,960</t>
@@ -866,25 +866,25 @@
     <t xml:space="preserve">65,495</t>
   </si>
   <si>
-    <t xml:space="preserve">(44,510; 85,625)</t>
+    <t xml:space="preserve">(44,510 to 85,625)</t>
   </si>
   <si>
     <t xml:space="preserve">65,045</t>
   </si>
   <si>
-    <t xml:space="preserve">(47,040; 81,970)</t>
+    <t xml:space="preserve">(47,040 to 81,970)</t>
   </si>
   <si>
     <t xml:space="preserve">69,225</t>
   </si>
   <si>
-    <t xml:space="preserve">(47,980; 89,670)</t>
+    <t xml:space="preserve">(47,980 to 89,670)</t>
   </si>
   <si>
     <t xml:space="preserve">10,865</t>
   </si>
   <si>
-    <t xml:space="preserve">(-3,425; 24,715)</t>
+    <t xml:space="preserve">(-3,425 to 24,715)</t>
   </si>
   <si>
     <t xml:space="preserve">10,110</t>
@@ -893,19 +893,19 @@
     <t xml:space="preserve">10,980</t>
   </si>
   <si>
-    <t xml:space="preserve">(-3,525; 24,785)</t>
+    <t xml:space="preserve">(-3,525 to 24,785)</t>
   </si>
   <si>
     <t xml:space="preserve">9,350</t>
   </si>
   <si>
-    <t xml:space="preserve">(-3,005; 21,775)</t>
+    <t xml:space="preserve">(-3,005 to 21,775)</t>
   </si>
   <si>
     <t xml:space="preserve">14,245</t>
   </si>
   <si>
-    <t xml:space="preserve">(-265; 28,120)</t>
+    <t xml:space="preserve">(-265 to 28,120)</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
matching output of table s1 to paper tables
</commit_message>
<xml_diff>
--- a/paper/Table_S1.xlsx
+++ b/paper/Table_S1.xlsx
@@ -50,247 +50,247 @@
     <t xml:space="preserve">Switzerland</t>
   </si>
   <si>
-    <t xml:space="preserve">1,380</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(-1,550 to 4,255)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1,100</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1,300</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(-1,650 to 4,130)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1,680</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(-865 to 4,190)</t>
+    <t xml:space="preserve">1 380</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(-1 550 to 4 255)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 100</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 300</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(-1 650 to 4 130)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 680</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(-865 to 4 190)</t>
   </si>
   <si>
     <t xml:space="preserve">-410</t>
   </si>
   <si>
-    <t xml:space="preserve">(-3,405 to 2,510)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3,455</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(705 to 6,120)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3,380</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3,360</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(605 to 6,015)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2,395</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(-310 to 5,020)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1,790</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(-1,110 to 4,565)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1,920</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(-1,265 to 5,010)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1,975</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1,585</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(-1,605 to 4,520)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1,950</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(-825 to 4,670)</t>
+    <t xml:space="preserve">(-3 405 to 2 510)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3 455</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(705 to 6 120)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3 380</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3 360</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(605 to 6 015)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2 395</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(-310 to 5 020)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 790</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(-1 110 to 4 565)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 920</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(-1 265 to 5 010)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 975</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 585</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(-1 605 to 4 520)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 950</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(-825 to 4 670)</t>
   </si>
   <si>
     <t xml:space="preserve">990</t>
   </si>
   <si>
-    <t xml:space="preserve">(-2,140 to 4,045)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3,810</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(1,155 to 6,395)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3,630</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3,855</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(1,175 to 6,505)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4,035</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(1,240 to 6,670)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1,905</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(-925 to 4,630)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">24,730</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(21,925 to 27,455)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">24,460</t>
-  </si>
-  <si>
-    <t xml:space="preserve">24,625</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(21,690 to 27,465)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">25,725</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(22,845 to 28,480)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">23,705</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(20,540 to 26,705)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3,730</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(510 to 6,835)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3,820</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3,700</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(515 to 6,790)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4,600</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(1,895 to 7,275)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(200 to 6,540)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1,535</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(-775 to 3,750)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1,555</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1,470</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(-865 to 3,725)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1,695</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(-505 to 3,905)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(-630 to 3,710)</t>
+    <t xml:space="preserve">(-2 140 to 4 045)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3 810</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(1 155 to 6 395)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3 630</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3 855</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(1 175 to 6 505)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4 035</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(1 240 to 6 670)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 905</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(-925 to 4 630)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">24 730</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(21 925 to 27 455)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">24 460</t>
+  </si>
+  <si>
+    <t xml:space="preserve">24 625</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(21 690 to 27 465)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">25 725</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(22 845 to 28 480)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">23 705</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(20 540 to 26 705)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3 730</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(510 to 6 835)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3 820</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3 700</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(515 to 6 790)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4 600</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(1 895 to 7 275)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(200 to 6 540)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 535</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(-775 to 3 750)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 555</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 470</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(-865 to 3 725)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 695</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(-505 to 3 905)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(-630 to 3 710)</t>
   </si>
   <si>
     <t xml:space="preserve">-920</t>
   </si>
   <si>
-    <t xml:space="preserve">(-3,680 to 1,805)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-1,200</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-1,035</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(-3,835 to 1,675)</t>
+    <t xml:space="preserve">(-3 680 to 1 805)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-1 200</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-1 035</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(-3 835 to 1 675)</t>
   </si>
   <si>
     <t xml:space="preserve">-180</t>
   </si>
   <si>
-    <t xml:space="preserve">(-2,650 to 2,250)</t>
+    <t xml:space="preserve">(-2 650 to 2 250)</t>
   </si>
   <si>
     <t xml:space="preserve">-25</t>
   </si>
   <si>
-    <t xml:space="preserve">(-2,440 to 2,295)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-3,705</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(-6,950 to -605)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-3,360</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-3,190</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(-6,315 to -185)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-2,980</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(-5,535 to -475)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-2,760</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(-5,095 to -380)</t>
+    <t xml:space="preserve">(-2 440 to 2 295)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-3 705</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(-6 950 to -605)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-3 360</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-3 190</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(-6 315 to -185)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-2 980</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(-5 535 to -475)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-2 760</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(-5 095 to -380)</t>
   </si>
   <si>
     <t xml:space="preserve">165</t>
   </si>
   <si>
-    <t xml:space="preserve">(-3,210 to 3,400)</t>
+    <t xml:space="preserve">(-3 210 to 3 400)</t>
   </si>
   <si>
     <t xml:space="preserve">280</t>
@@ -299,52 +299,52 @@
     <t xml:space="preserve">320</t>
   </si>
   <si>
-    <t xml:space="preserve">(-2,950 to 3,460)</t>
+    <t xml:space="preserve">(-2 950 to 3 460)</t>
   </si>
   <si>
     <t xml:space="preserve">395</t>
   </si>
   <si>
-    <t xml:space="preserve">(-2,200 to 2,895)</t>
+    <t xml:space="preserve">(-2 200 to 2 895)</t>
   </si>
   <si>
     <t xml:space="preserve">600</t>
   </si>
   <si>
-    <t xml:space="preserve">(-1,865 to 2,975)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">8,430</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(5,255 to 11,450)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">8,810</t>
-  </si>
-  <si>
-    <t xml:space="preserve">8,685</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(5,575 to 11,675)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">8,105</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(5,505 to 10,630)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">7,360</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(4,395 to 10,240)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-1,000</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(-3,085 to 955)</t>
+    <t xml:space="preserve">(-1 865 to 2 975)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8 430</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(5 255 to 11 450)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8 810</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8 685</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(5 575 to 11 675)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8 105</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(5 505 to 10 630)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7 360</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(4 395 to 10 240)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-1 000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(-3 085 to 955)</t>
   </si>
   <si>
     <t xml:space="preserve">-845</t>
@@ -353,559 +353,559 @@
     <t xml:space="preserve">-715</t>
   </si>
   <si>
-    <t xml:space="preserve">(-2,735 to 1,220)</t>
+    <t xml:space="preserve">(-2 735 to 1 220)</t>
   </si>
   <si>
     <t xml:space="preserve">-795</t>
   </si>
   <si>
-    <t xml:space="preserve">(-2,715 to 1,010)</t>
+    <t xml:space="preserve">(-2 715 to 1 010)</t>
   </si>
   <si>
     <t xml:space="preserve">-925</t>
   </si>
   <si>
-    <t xml:space="preserve">(-3,280 to 1,375)</t>
+    <t xml:space="preserve">(-3 280 to 1 375)</t>
   </si>
   <si>
     <t xml:space="preserve">Sweden</t>
   </si>
   <si>
-    <t xml:space="preserve">2,495</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(-1,400 to 6,155)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2,785</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2,540</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(-1,280 to 6,290)</t>
+    <t xml:space="preserve">2 495</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(-1 400 to 6 155)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2 785</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2 540</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(-1 280 to 6 290)</t>
   </si>
   <si>
     <t xml:space="preserve">290</t>
   </si>
   <si>
-    <t xml:space="preserve">(-3,385 to 3,790)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-1,125</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(-5,425 to 2,960)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(4,870 to 12,575)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">8,720</t>
-  </si>
-  <si>
-    <t xml:space="preserve">8,525</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(4,475 to 12,495)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">7,380</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(3,750 to 10,945)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">7,060</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(2,930 to 11,055)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5,295</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(800 to 9,480)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6,365</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5,570</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(1,045 to 9,800)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6,515</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(2,655 to 10,245)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5,875</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(1,405 to 10,255)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-2,640</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(-7,970 to 2,330)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-2,865</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(-8,140 to 2,105)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-2,945</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(-7,240 to 1,245)</t>
+    <t xml:space="preserve">(-3 385 to 3 790)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-1 125</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(-5 425 to 2 960)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(4 870 to 12 575)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8 720</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8 525</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(4 475 to 12 495)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7 380</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(3 750 to 10 945)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7 060</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(2 930 to 11 055)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5 295</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(800 to 9 480)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6 365</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5 570</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(1 045 to 9 800)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6 515</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(2 655 to 10 245)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5 875</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(1 405 to 10 255)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-2 640</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(-7 970 to 2 330)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-2 865</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(-8 140 to 2 105)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-2 945</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(-7 240 to 1 245)</t>
   </si>
   <si>
     <t xml:space="preserve">-645</t>
   </si>
   <si>
-    <t xml:space="preserve">(-4,165 to 2,725)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">25,935</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(20,595 to 31,085)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">25,505</t>
-  </si>
-  <si>
-    <t xml:space="preserve">25,695</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(20,310 to 30,885)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">25,735</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(21,420 to 29,845)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">27,700</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(23,945 to 31,250)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">7,245</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(1,180 to 12,965)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">8,260</t>
-  </si>
-  <si>
-    <t xml:space="preserve">7,140</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(1,020 to 12,835)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(1,265 to 10,350)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">7,395</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(3,625 to 11,080)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1,080</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(-2,395 to 4,445)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1,450</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(-2,085 to 4,910)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1,050</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(-1,825 to 3,820)</t>
+    <t xml:space="preserve">(-4 165 to 2 725)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">25 935</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(20 595 to 31 085)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">25 505</t>
+  </si>
+  <si>
+    <t xml:space="preserve">25 695</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(20 310 to 30 885)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">25 735</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(21 420 to 29 845)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">27 700</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(23 945 to 31 250)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7 245</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(1 180 to 12 965)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8 260</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7 140</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(1 020 to 12 835)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(1 265 to 10 350)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7 395</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(3 625 to 11 080)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 080</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(-2 395 to 4 445)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 450</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(-2 085 to 4 910)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 050</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(-1 825 to 3 820)</t>
   </si>
   <si>
     <t xml:space="preserve">880</t>
   </si>
   <si>
-    <t xml:space="preserve">(-2,410 to 4,065)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2,760</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(100 to 5,340)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3,040</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2,990</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(395 to 5,515)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3,325</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(410 to 6,220)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3,135</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(-470 to 6,575)</t>
+    <t xml:space="preserve">(-2 410 to 4 065)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2 760</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(100 to 5 340)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3 040</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2 990</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(395 to 5 515)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3 325</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(410 to 6 220)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3 135</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(-470 to 6 575)</t>
   </si>
   <si>
     <t xml:space="preserve">-360</t>
   </si>
   <si>
-    <t xml:space="preserve">(-3,505 to 2,720)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1,040</t>
+    <t xml:space="preserve">(-3 505 to 2 720)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 040</t>
   </si>
   <si>
     <t xml:space="preserve">620</t>
   </si>
   <si>
-    <t xml:space="preserve">(-2,465 to 3,605)</t>
+    <t xml:space="preserve">(-2 465 to 3 605)</t>
   </si>
   <si>
     <t xml:space="preserve">-315</t>
   </si>
   <si>
-    <t xml:space="preserve">(-3,565 to 2,800)</t>
+    <t xml:space="preserve">(-3 565 to 2 800)</t>
   </si>
   <si>
     <t xml:space="preserve">-800</t>
   </si>
   <si>
-    <t xml:space="preserve">(-4,875 to 3,060)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-4,365</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(-8,015 to -795)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-4,390</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-4,255</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(-7,810 to -730)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-3,350</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(-6,330 to -345)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-4,380</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(-7,125 to -1,695)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">7,655</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(4,200 to 10,985)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">8,465</t>
-  </si>
-  <si>
-    <t xml:space="preserve">8,405</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(4,960 to 11,690)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6,760</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(3,635 to 9,910)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2,600</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(-690 to 5,750)</t>
+    <t xml:space="preserve">(-4 875 to 3 060)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-4 365</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(-8 015 to -795)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-4 390</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-4 255</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(-7 810 to -730)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-3 350</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(-6 330 to -345)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-4 380</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(-7 125 to -1 695)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7 655</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(4 200 to 10 985)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8 465</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8 405</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(4 960 to 11 690)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6 760</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(3 635 to 9 910)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2 600</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(-690 to 5 750)</t>
   </si>
   <si>
     <t xml:space="preserve">--</t>
   </si>
   <si>
-    <t xml:space="preserve">1,700</t>
+    <t xml:space="preserve">1 700</t>
   </si>
   <si>
     <t xml:space="preserve">750</t>
   </si>
   <si>
-    <t xml:space="preserve">(-1,845 to 3,160)</t>
+    <t xml:space="preserve">(-1 845 to 3 160)</t>
   </si>
   <si>
     <t xml:space="preserve">Spain</t>
   </si>
   <si>
-    <t xml:space="preserve">11,645</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(-13,875 to 36,180)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">12,155</t>
-  </si>
-  <si>
-    <t xml:space="preserve">12,020</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(-13,400 to 36,025)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">22,060</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(-900 to 44,430)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">20,950</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(1,005 to 40,565)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">241,660</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(215,790 to 266,105)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">239,680</t>
-  </si>
-  <si>
-    <t xml:space="preserve">239,495</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(214,035 to 264,175)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">243,240</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(218,610 to 266,700)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">28,835</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(1,100 to 55,560)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">23,340</t>
-  </si>
-  <si>
-    <t xml:space="preserve">22,835</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(-4,940 to 49,265)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">24,670</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(-165 to 48,125)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">45,235</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(21,520 to 67,910)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">32,305</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(9,145 to 53,685)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">39,455</t>
-  </si>
-  <si>
-    <t xml:space="preserve">33,085</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(10,205 to 54,805)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">33,355</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(14,275 to 51,825)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">30,730</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(15,545 to 45,480)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">13,225</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(-2,660 to 28,785)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10,715</t>
-  </si>
-  <si>
-    <t xml:space="preserve">11,675</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(-4,495 to 27,310)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">28,360</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(7,820 to 48,025)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">21,360</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(4,365 to 37,570)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-28,160</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(-47,480 to -9,435)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-32,630</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-28,615</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(-48,745 to -9,615)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-11,425</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(-33,630 to 9,845)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-27,265</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(-44,020 to -10,910)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-13,370</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(-34,800 to 7,185)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-20,505</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-19,885</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(-41,320 to 1,025)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-8,505</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(-26,810 to 9,205)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-10,460</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(-31,415 to 9,695)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">72,330</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(51,940 to 92,410)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">65,960</t>
-  </si>
-  <si>
-    <t xml:space="preserve">65,495</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(44,510 to 85,625)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">65,045</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(47,040 to 81,970)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">69,225</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(47,980 to 89,670)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10,865</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(-3,425 to 24,715)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10,110</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10,980</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(-3,525 to 24,785)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">9,350</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(-3,005 to 21,775)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">14,245</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(-265 to 28,120)</t>
+    <t xml:space="preserve">11 645</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(-13 875 to 36 180)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12 155</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12 020</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(-13 400 to 36 025)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">22 060</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(-900 to 44 430)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20 950</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(1 005 to 40 565)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">241 660</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(215 790 to 266 105)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">239 680</t>
+  </si>
+  <si>
+    <t xml:space="preserve">239 495</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(214 035 to 264 175)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">243 240</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(218 610 to 266 700)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">28 835</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(1 100 to 55 560)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">23 340</t>
+  </si>
+  <si>
+    <t xml:space="preserve">22 835</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(-4 940 to 49 265)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">24 670</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(-165 to 48 125)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">45 235</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(21 520 to 67 910)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">32 305</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(9 145 to 53 685)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">39 455</t>
+  </si>
+  <si>
+    <t xml:space="preserve">33 085</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(10 205 to 54 805)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">33 355</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(14 275 to 51 825)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">30 730</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(15 545 to 45 480)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">13 225</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(-2 660 to 28 785)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10 715</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11 675</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(-4 495 to 27 310)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">28 360</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(7 820 to 48 025)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">21 360</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(4 365 to 37 570)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-28 160</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(-47 480 to -9 435)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-32 630</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-28 615</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(-48 745 to -9 615)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-11 425</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(-33 630 to 9 845)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-27 265</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(-44 020 to -10 910)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-13 370</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(-34 800 to 7 185)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-20 505</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-19 885</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(-41 320 to 1 025)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-8 505</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(-26 810 to 9 205)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-10 460</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(-31 415 to 9 695)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">72 330</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(51 940 to 92 410)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">65 960</t>
+  </si>
+  <si>
+    <t xml:space="preserve">65 495</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(44 510 to 85 625)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">65 045</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(47 040 to 81 970)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">69 225</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(47 980 to 89 670)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10 865</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(-3 425 to 24 715)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10 110</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10 980</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(-3 525 to 24 785)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9 350</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(-3 005 to 21 775)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">14 245</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(-265 to 28 120)</t>
   </si>
 </sst>
 </file>

</xml_diff>